<commit_message>
section 127 data exploration
</commit_message>
<xml_diff>
--- a/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
+++ b/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\research-dissertation-case-for-alt-ed\papers\section-127-effects\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4E81AA57-1489-45DB-90D5-C03FE1237E85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6899D18-C1CC-489D-95FB-0F0F0E37A09F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="section-127-effects" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Year</t>
   </si>
@@ -75,11 +83,20 @@
   <si>
     <t>Special Delta</t>
   </si>
+  <si>
+    <t>Total Enrollment</t>
+  </si>
+  <si>
+    <t>Public Enrollment</t>
+  </si>
+  <si>
+    <t>New H-1 Visa Award</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -557,8 +574,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -913,11 +931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,11 +943,12 @@
     <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -955,25 +974,34 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -1002,15 +1030,21 @@
       <c r="H2">
         <v>4203</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>25.7</v>
       </c>
-      <c r="M2">
-        <f>AVERAGE(I2:I6)</f>
-        <v>25.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K2" s="1">
+        <v>8580887</v>
+      </c>
+      <c r="L2" s="1">
+        <v>6428134</v>
+      </c>
+      <c r="P2" s="1">
+        <f>AVERAGE(L2:L6)</f>
+        <v>7142218.7999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -1039,11 +1073,17 @@
       <c r="H3">
         <v>4268</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K3" s="1">
+        <v>8948644</v>
+      </c>
+      <c r="L3" s="1">
+        <v>6804309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -1072,11 +1112,17 @@
       <c r="H4">
         <v>4305</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K4" s="1">
+        <v>9214860</v>
+      </c>
+      <c r="L4" s="1">
+        <v>7070635</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -1105,18 +1151,24 @@
       <c r="H5">
         <v>4141</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>24</v>
       </c>
-      <c r="J5">
-        <f>AVERAGE(I5:I9)</f>
-        <v>25.540000000000003</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1">
+        <v>9602123</v>
+      </c>
+      <c r="L5" s="1">
+        <v>7419516</v>
+      </c>
+      <c r="M5" s="1">
+        <f>AVERAGE(L5:L9)</f>
+        <v>8348598.7999999998</v>
+      </c>
+      <c r="N5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -1145,11 +1197,17 @@
       <c r="H6">
         <v>3792</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K6" s="1">
+        <v>10223729</v>
+      </c>
+      <c r="L6" s="1">
+        <v>7988500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -1178,19 +1236,25 @@
       <c r="H7">
         <v>3628</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>26.3</v>
       </c>
-      <c r="M7">
-        <f t="shared" ref="M7" si="4">AVERAGE(I7:I11)</f>
-        <v>25.879999999999995</v>
-      </c>
-      <c r="N7">
-        <f>M7-M2</f>
-        <v>0.67999999999999616</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K7" s="1">
+        <v>11184859</v>
+      </c>
+      <c r="L7" s="1">
+        <v>8834508</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" ref="P7" si="4">AVERAGE(L7:L11)</f>
+        <v>8831538.5999999996</v>
+      </c>
+      <c r="Q7">
+        <f>P7-P2</f>
+        <v>1689319.7999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -1219,11 +1283,17 @@
       <c r="H8">
         <v>3820</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>26.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K8" s="1">
+        <v>11012137</v>
+      </c>
+      <c r="L8" s="1">
+        <v>8653477</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -1252,11 +1322,17 @@
       <c r="H9">
         <v>3814</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>11285787</v>
+      </c>
+      <c r="L9" s="1">
+        <v>8846993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -1285,22 +1361,28 @@
       <c r="H10">
         <v>3800</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>25.3</v>
       </c>
-      <c r="J10">
-        <f>AVERAGE(I10:I14)</f>
-        <v>25.74</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1">
+        <v>11260092</v>
+      </c>
+      <c r="L10" s="1">
+        <v>8785893</v>
+      </c>
+      <c r="M10" s="1">
+        <f>AVERAGE(L10:L14)</f>
+        <v>9324645.5999999996</v>
+      </c>
+      <c r="N10" t="s">
         <v>9</v>
       </c>
-      <c r="L10">
-        <f>J10-J5</f>
-        <v>0.19999999999999574</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <f>M10-M5</f>
+        <v>976046.79999999981</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -1329,11 +1411,17 @@
       <c r="H11">
         <v>3635</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K11" s="1">
+        <v>11569899</v>
+      </c>
+      <c r="L11" s="1">
+        <v>9036822</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -1362,19 +1450,25 @@
       <c r="H12">
         <v>3610</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>25.7</v>
       </c>
-      <c r="M12">
-        <f t="shared" ref="M12" si="5">AVERAGE(I12:I16)</f>
-        <v>26.340000000000003</v>
-      </c>
-      <c r="N12">
-        <f t="shared" ref="N12" si="6">M12-M7</f>
-        <v>0.46000000000000796</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K12" s="1">
+        <v>12096895</v>
+      </c>
+      <c r="L12" s="1">
+        <v>9457394</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" ref="P12" si="5">AVERAGE(L12:L16)</f>
+        <v>9592123.4000000004</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12" si="6">P12-P7</f>
+        <v>760584.80000000075</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -1403,18 +1497,24 @@
       <c r="H13">
         <v>3765</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>26.1</v>
       </c>
-      <c r="J13">
-        <f>AVERAGE(I13:I17)</f>
-        <v>26.76</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="K13" s="1">
+        <v>12371672</v>
+      </c>
+      <c r="L13" s="1">
+        <v>9647032</v>
+      </c>
+      <c r="M13" s="1">
+        <f>AVERAGE(L13:L17)</f>
+        <v>9596499.1999999993</v>
+      </c>
+      <c r="N13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1982</v>
       </c>
@@ -1443,11 +1543,17 @@
       <c r="H14">
         <v>4020</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K14" s="1">
+        <v>12425780</v>
+      </c>
+      <c r="L14" s="1">
+        <v>9696087</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1983</v>
       </c>
@@ -1476,11 +1582,17 @@
       <c r="H15">
         <v>4250</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K15" s="1">
+        <v>12464661</v>
+      </c>
+      <c r="L15" s="1">
+        <v>9682734</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1984</v>
       </c>
@@ -1509,11 +1621,17 @@
       <c r="H16">
         <v>4555</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>27.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K16" s="1">
+        <v>12241940</v>
+      </c>
+      <c r="L16" s="1">
+        <v>9477370</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1985</v>
       </c>
@@ -1542,19 +1660,25 @@
       <c r="H17">
         <v>4864</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>27.8</v>
       </c>
-      <c r="M17">
-        <f t="shared" ref="M17" si="7">AVERAGE(I17:I21)</f>
-        <v>29.3</v>
-      </c>
-      <c r="N17">
-        <f t="shared" ref="N17" si="8">M17-M12</f>
-        <v>2.9599999999999973</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K17" s="1">
+        <v>12247055</v>
+      </c>
+      <c r="L17" s="1">
+        <v>9479273</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" ref="P17" si="7">AVERAGE(L17:L21)</f>
+        <v>9981154.1999999993</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" ref="Q17" si="8">P17-P12</f>
+        <v>389030.79999999888</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1986</v>
       </c>
@@ -1583,22 +1707,28 @@
       <c r="H18">
         <v>5044</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>27.9</v>
       </c>
-      <c r="J18">
-        <f>AVERAGE(I18:I22)</f>
-        <v>30.139999999999997</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="K18" s="1">
+        <v>12503511</v>
+      </c>
+      <c r="L18" s="1">
+        <v>9713893</v>
+      </c>
+      <c r="M18" s="1">
+        <f>AVERAGE(L18:L22)</f>
+        <v>10254243</v>
+      </c>
+      <c r="N18" t="s">
         <v>10</v>
       </c>
-      <c r="L18">
-        <f>J18-J13</f>
-        <v>3.3799999999999955</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f>M18-M13</f>
+        <v>657743.80000000075</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1987</v>
       </c>
@@ -1627,11 +1757,17 @@
       <c r="H19">
         <v>5149</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>29.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K19" s="1">
+        <v>12766642</v>
+      </c>
+      <c r="L19" s="1">
+        <v>9973254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1988</v>
       </c>
@@ -1660,11 +1796,17 @@
       <c r="H20">
         <v>5321</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>30.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K20" s="1">
+        <v>13055337</v>
+      </c>
+      <c r="L20" s="1">
+        <v>10161388</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1989</v>
       </c>
@@ -1693,11 +1835,17 @@
       <c r="H21">
         <v>5426</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>30.9</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K21" s="1">
+        <v>13538560</v>
+      </c>
+      <c r="L21" s="1">
+        <v>10577963</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1990</v>
       </c>
@@ -1727,18 +1875,27 @@
         <v>5465</v>
       </c>
       <c r="I22">
+        <v>794</v>
+      </c>
+      <c r="J22">
         <v>32</v>
       </c>
-      <c r="M22">
-        <f t="shared" ref="M22" si="9">AVERAGE(I22:I26)</f>
-        <v>33.659999999999997</v>
-      </c>
-      <c r="N22">
-        <f t="shared" ref="N22" si="10">M22-M17</f>
-        <v>4.3599999999999959</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K22" s="1">
+        <v>13818637</v>
+      </c>
+      <c r="L22" s="1">
+        <v>10844717</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" ref="P22" si="9">AVERAGE(L22:L26)</f>
+        <v>11172323</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" ref="Q22" si="10">P22-P17</f>
+        <v>1191168.8000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1991</v>
       </c>
@@ -1768,10 +1925,19 @@
         <v>5768</v>
       </c>
       <c r="I23">
+        <v>51882</v>
+      </c>
+      <c r="J23">
         <v>33.299999999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K23" s="1">
+        <v>14358953</v>
+      </c>
+      <c r="L23" s="1">
+        <v>11309563</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1992</v>
       </c>
@@ -1801,10 +1967,19 @@
         <v>5988</v>
       </c>
       <c r="I24">
+        <v>44290</v>
+      </c>
+      <c r="J24">
         <v>34.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K24" s="1">
+        <v>14487359</v>
+      </c>
+      <c r="L24" s="1">
+        <v>11384567</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1993</v>
       </c>
@@ -1834,10 +2009,19 @@
         <v>6352</v>
       </c>
       <c r="I25">
+        <v>35818</v>
+      </c>
+      <c r="J25">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K25" s="1">
+        <v>14304803</v>
+      </c>
+      <c r="L25" s="1">
+        <v>11189088</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1994</v>
       </c>
@@ -1867,10 +2051,19 @@
         <v>6525</v>
       </c>
       <c r="I26">
+        <v>42843</v>
+      </c>
+      <c r="J26">
         <v>34.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K26" s="1">
+        <v>14278790</v>
+      </c>
+      <c r="L26" s="1">
+        <v>11133680</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1995</v>
       </c>
@@ -1900,18 +2093,27 @@
         <v>6813</v>
       </c>
       <c r="I27">
+        <v>51832</v>
+      </c>
+      <c r="J27">
         <v>34.299999999999997</v>
       </c>
-      <c r="M27">
-        <f t="shared" ref="M27" si="11">AVERAGE(I27:I31)</f>
-        <v>35.739999999999995</v>
-      </c>
-      <c r="N27">
-        <f t="shared" ref="N27" si="12">M27-M22</f>
-        <v>2.0799999999999983</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K27" s="1">
+        <v>14261781</v>
+      </c>
+      <c r="L27" s="1">
+        <v>11092374</v>
+      </c>
+      <c r="P27" s="1">
+        <f t="shared" ref="P27" si="11">AVERAGE(L27:L31)</f>
+        <v>11184500</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" ref="Q27" si="12">P27-P22</f>
+        <v>12177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1996</v>
       </c>
@@ -1941,10 +2143,19 @@
         <v>6970</v>
       </c>
       <c r="I28">
+        <v>58327</v>
+      </c>
+      <c r="J28">
         <v>35.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K28" s="1">
+        <v>14367520</v>
+      </c>
+      <c r="L28" s="1">
+        <v>11120499</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1997</v>
       </c>
@@ -1974,10 +2185,19 @@
         <v>7133</v>
       </c>
       <c r="I29">
+        <v>80547</v>
+      </c>
+      <c r="J29">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K29" s="1">
+        <v>14502334</v>
+      </c>
+      <c r="L29" s="1">
+        <v>11196119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1998</v>
       </c>
@@ -2007,10 +2227,19 @@
         <v>7393</v>
       </c>
       <c r="I30">
+        <v>91360</v>
+      </c>
+      <c r="J30">
         <v>36.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K30" s="1">
+        <v>14506967</v>
+      </c>
+      <c r="L30" s="1">
+        <v>11137769</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1999</v>
       </c>
@@ -2040,10 +2269,19 @@
         <v>7485</v>
       </c>
       <c r="I31">
+        <v>116513</v>
+      </c>
+      <c r="J31">
         <v>35.6</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K31" s="1">
+        <v>14849691</v>
+      </c>
+      <c r="L31" s="1">
+        <v>11375739</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -2073,18 +2311,27 @@
         <v>7452</v>
       </c>
       <c r="I32">
+        <v>133290</v>
+      </c>
+      <c r="J32">
         <v>35.5</v>
       </c>
-      <c r="M32">
-        <f t="shared" ref="M32" si="13">AVERAGE(I32:I36)</f>
-        <v>36.86</v>
-      </c>
-      <c r="N32">
-        <f t="shared" ref="N32" si="14">M32-M27</f>
-        <v>1.1200000000000045</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K32" s="1">
+        <v>15312289</v>
+      </c>
+      <c r="L32" s="1">
+        <v>11752786</v>
+      </c>
+      <c r="P32" s="1">
+        <f t="shared" ref="P32" si="13">AVERAGE(L32:L36)</f>
+        <v>12515349</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" ref="Q32" si="14">P32-P27</f>
+        <v>1330849</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -2114,10 +2361,19 @@
         <v>7689</v>
       </c>
       <c r="I33">
+        <v>161643</v>
+      </c>
+      <c r="J33">
         <v>36.299999999999997</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K33" s="1">
+        <v>15927987</v>
+      </c>
+      <c r="L33" s="1">
+        <v>12233156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2002</v>
       </c>
@@ -2147,10 +2403,19 @@
         <v>7998</v>
       </c>
       <c r="I34">
+        <v>118352</v>
+      </c>
+      <c r="J34">
         <v>36.700000000000003</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K34" s="1">
+        <v>16611711</v>
+      </c>
+      <c r="L34" s="1">
+        <v>12751993</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2003</v>
       </c>
@@ -2180,10 +2445,19 @@
         <v>8617</v>
       </c>
       <c r="I35">
+        <v>107196</v>
+      </c>
+      <c r="J35">
         <v>37.799999999999997</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K35" s="1">
+        <v>16911481</v>
+      </c>
+      <c r="L35" s="1">
+        <v>12858698</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2004</v>
       </c>
@@ -2213,10 +2487,19 @@
         <v>9016</v>
       </c>
       <c r="I36">
+        <v>139037</v>
+      </c>
+      <c r="J36">
         <v>38</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K36" s="1">
+        <v>17272044</v>
+      </c>
+      <c r="L36" s="1">
+        <v>12980112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2005</v>
       </c>
@@ -2246,18 +2529,27 @@
         <v>9269</v>
       </c>
       <c r="I37">
+        <v>124374</v>
+      </c>
+      <c r="J37">
         <v>38.9</v>
       </c>
-      <c r="M37">
-        <f t="shared" ref="M37" si="15">AVERAGE(I37:I41)</f>
-        <v>39.179999999999993</v>
-      </c>
-      <c r="N37">
-        <f t="shared" ref="N37" si="16">M37-M32</f>
-        <v>2.3199999999999932</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K37" s="1">
+        <v>17487475</v>
+      </c>
+      <c r="L37" s="1">
+        <v>13021834</v>
+      </c>
+      <c r="P37" s="1">
+        <f t="shared" ref="P37" si="15">AVERAGE(L37:L41)</f>
+        <v>13695941.6</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" ref="Q37" si="16">P37-P32</f>
+        <v>1180592.5999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2006</v>
       </c>
@@ -2287,10 +2579,19 @@
         <v>9619</v>
       </c>
       <c r="I38">
+        <v>135861</v>
+      </c>
+      <c r="J38">
         <v>37.299999999999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K38" s="1">
+        <v>17754230</v>
+      </c>
+      <c r="L38" s="1">
+        <v>13175350</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2007</v>
       </c>
@@ -2320,10 +2621,19 @@
         <v>9724</v>
       </c>
       <c r="I39">
+        <v>154692</v>
+      </c>
+      <c r="J39">
         <v>38.799999999999997</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K39" s="1">
+        <v>18258138</v>
+      </c>
+      <c r="L39" s="1">
+        <v>13500894</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2008</v>
       </c>
@@ -2353,10 +2663,19 @@
         <v>10052</v>
       </c>
       <c r="I40">
+        <v>130183</v>
+      </c>
+      <c r="J40">
         <v>39.6</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K40" s="1">
+        <v>19081686</v>
+      </c>
+      <c r="L40" s="1">
+        <v>13970862</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2009</v>
       </c>
@@ -2386,10 +2705,19 @@
         <v>10227</v>
       </c>
       <c r="I41">
+        <v>110988</v>
+      </c>
+      <c r="J41">
         <v>41.3</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K41" s="1">
+        <v>20313594</v>
+      </c>
+      <c r="L41" s="1">
+        <v>14810768</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2010</v>
       </c>
@@ -2419,18 +2747,27 @@
         <v>10509</v>
       </c>
       <c r="I42">
+        <v>117828</v>
+      </c>
+      <c r="J42">
         <v>41.2</v>
       </c>
-      <c r="M42">
-        <f t="shared" ref="M42" si="17">AVERAGE(I42:I46)</f>
-        <v>40.82</v>
-      </c>
-      <c r="N42">
-        <f t="shared" ref="N42" si="18">M42-M37</f>
-        <v>1.6400000000000077</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K42" s="1">
+        <v>21019438</v>
+      </c>
+      <c r="L42" s="1">
+        <v>15142171</v>
+      </c>
+      <c r="P42" s="1">
+        <f t="shared" ref="P42" si="17">AVERAGE(L42:L46)</f>
+        <v>14908929.800000001</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" ref="Q42" si="18">P42-P37</f>
+        <v>1212988.2000000011</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -2460,10 +2797,19 @@
         <v>10854</v>
       </c>
       <c r="I43">
+        <v>129552</v>
+      </c>
+      <c r="J43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K43" s="1">
+        <v>21010590</v>
+      </c>
+      <c r="L43" s="1">
+        <v>15116303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2012</v>
       </c>
@@ -2493,10 +2839,19 @@
         <v>11203</v>
       </c>
       <c r="I44">
+        <v>135991</v>
+      </c>
+      <c r="J44">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K44" s="1">
+        <v>20644478</v>
+      </c>
+      <c r="L44" s="1">
+        <v>14884667</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2013</v>
       </c>
@@ -2526,10 +2881,19 @@
         <v>11435</v>
       </c>
       <c r="I45">
+        <v>153794</v>
+      </c>
+      <c r="J45">
         <v>39.9</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K45" s="1">
+        <v>20376677</v>
+      </c>
+      <c r="L45" s="1">
+        <v>14746848</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2014</v>
       </c>
@@ -2559,10 +2923,19 @@
         <v>11778</v>
       </c>
       <c r="I46">
+        <v>162239</v>
+      </c>
+      <c r="J46">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K46" s="1">
+        <v>20209092</v>
+      </c>
+      <c r="L46" s="1">
+        <v>14654660</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2015</v>
       </c>
@@ -2592,18 +2965,27 @@
         <v>12080</v>
       </c>
       <c r="I47">
+        <v>173799</v>
+      </c>
+      <c r="J47">
         <v>40.5</v>
       </c>
-      <c r="M47">
-        <f t="shared" ref="M47" si="19">AVERAGE(I47:I51)</f>
-        <v>40.85</v>
-      </c>
-      <c r="N47">
-        <f t="shared" ref="N47" si="20">M47-M42</f>
-        <v>3.0000000000001137E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K47" s="1">
+        <v>19988204</v>
+      </c>
+      <c r="L47" s="1">
+        <v>14572843</v>
+      </c>
+      <c r="P47" s="1">
+        <f t="shared" ref="P47" si="19">AVERAGE(L47:L51)</f>
+        <v>14572946</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" ref="Q47" si="20">P47-P42</f>
+        <v>-335983.80000000075</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2016</v>
       </c>
@@ -2633,7 +3015,40 @@
         <v>12219</v>
       </c>
       <c r="I48">
+        <v>181351</v>
+      </c>
+      <c r="J48">
         <v>41.2</v>
+      </c>
+      <c r="K48" s="1">
+        <v>19846904</v>
+      </c>
+      <c r="L48" s="1">
+        <v>14585840</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2017</v>
+      </c>
+      <c r="B49">
+        <v>5250</v>
+      </c>
+      <c r="C49">
+        <f>B49*($G$48/G49)</f>
+        <v>4781.1422887206982</v>
+      </c>
+      <c r="G49">
+        <v>13998.65</v>
+      </c>
+      <c r="I49">
+        <v>180440</v>
+      </c>
+      <c r="K49" s="1">
+        <v>19765598</v>
+      </c>
+      <c r="L49">
+        <v>14560155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stafford loan and gi bill into regression
</commit_message>
<xml_diff>
--- a/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
+++ b/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\research-dissertation-case-for-alt-ed\papers\section-127-effects\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6899D18-C1CC-489D-95FB-0F0F0E37A09F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACA265C-D02F-4A40-B766-1DBFA5B3639B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
   <si>
     <t>Year</t>
   </si>
@@ -91,6 +91,30 @@
   </si>
   <si>
     <t>New H-1 Visa Award</t>
+  </si>
+  <si>
+    <t>Stafford Limit for Undergraduates</t>
+  </si>
+  <si>
+    <t>Stafford Limit is Combined Subsidized and Unsubsidized</t>
+  </si>
+  <si>
+    <t>GI Education Benefit State</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -932,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,12 +967,12 @@
     <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.85546875" customWidth="1"/>
+    <col min="4" max="12" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -977,31 +1001,40 @@
         <v>20</v>
       </c>
       <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -1031,20 +1064,30 @@
         <v>4203</v>
       </c>
       <c r="J2">
+        <f>1500*4</f>
+        <v>6000</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2">
         <v>25.7</v>
       </c>
-      <c r="K2" s="1">
+      <c r="N2" s="1">
         <v>8580887</v>
       </c>
-      <c r="L2" s="1">
+      <c r="O2" s="1">
         <v>6428134</v>
       </c>
-      <c r="P2" s="1">
-        <f>AVERAGE(L2:L6)</f>
+      <c r="S2" s="1">
+        <f>AVERAGE(O2:O6)</f>
         <v>7142218.7999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -1074,16 +1117,26 @@
         <v>4268</v>
       </c>
       <c r="J3">
+        <f t="shared" ref="J3:J4" si="4">1500*4</f>
+        <v>6000</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3">
         <v>26.2</v>
       </c>
-      <c r="K3" s="1">
+      <c r="N3" s="1">
         <v>8948644</v>
       </c>
-      <c r="L3" s="1">
+      <c r="O3" s="1">
         <v>6804309</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -1113,16 +1166,26 @@
         <v>4305</v>
       </c>
       <c r="J4">
+        <f t="shared" si="4"/>
+        <v>6000</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4">
         <v>25.5</v>
       </c>
-      <c r="K4" s="1">
+      <c r="N4" s="1">
         <v>9214860</v>
       </c>
-      <c r="L4" s="1">
+      <c r="O4" s="1">
         <v>7070635</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -1152,23 +1215,33 @@
         <v>4141</v>
       </c>
       <c r="J5">
+        <f>100+1500+2500+2500</f>
+        <v>6600</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="1">
+      <c r="M5">
+        <v>24</v>
+      </c>
+      <c r="N5" s="1">
         <v>9602123</v>
       </c>
-      <c r="L5" s="1">
+      <c r="O5" s="1">
         <v>7419516</v>
       </c>
-      <c r="M5" s="1">
-        <f>AVERAGE(L5:L9)</f>
+      <c r="P5" s="1">
+        <f>AVERAGE(O5:O9)</f>
         <v>8348598.7999999998</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -1198,16 +1271,26 @@
         <v>3792</v>
       </c>
       <c r="J6">
+        <f t="shared" ref="J6:J8" si="5">100+1500+2500+2500</f>
+        <v>6600</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6">
         <v>24.6</v>
       </c>
-      <c r="K6" s="1">
+      <c r="N6" s="1">
         <v>10223729</v>
       </c>
-      <c r="L6" s="1">
+      <c r="O6" s="1">
         <v>7988500</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -1237,24 +1320,34 @@
         <v>3628</v>
       </c>
       <c r="J7">
+        <f t="shared" si="5"/>
+        <v>6600</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7">
         <v>26.3</v>
       </c>
-      <c r="K7" s="1">
+      <c r="N7" s="1">
         <v>11184859</v>
       </c>
-      <c r="L7" s="1">
+      <c r="O7" s="1">
         <v>8834508</v>
       </c>
-      <c r="P7" s="1">
-        <f t="shared" ref="P7" si="4">AVERAGE(L7:L11)</f>
+      <c r="S7" s="1">
+        <f t="shared" ref="S7" si="6">AVERAGE(O7:O11)</f>
         <v>8831538.5999999996</v>
       </c>
-      <c r="Q7">
-        <f>P7-P2</f>
+      <c r="T7">
+        <f>S7-S2</f>
         <v>1689319.7999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -1284,16 +1377,26 @@
         <v>3820</v>
       </c>
       <c r="J8">
+        <f t="shared" si="5"/>
+        <v>6600</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8">
         <v>26.7</v>
       </c>
-      <c r="K8" s="1">
+      <c r="N8" s="1">
         <v>11012137</v>
       </c>
-      <c r="L8" s="1">
+      <c r="O8" s="1">
         <v>8653477</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -1323,16 +1426,26 @@
         <v>3814</v>
       </c>
       <c r="J9">
+        <f>2500*4</f>
+        <v>10000</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9">
         <v>26.1</v>
       </c>
-      <c r="K9" s="1">
+      <c r="N9" s="1">
         <v>11285787</v>
       </c>
-      <c r="L9" s="1">
+      <c r="O9" s="1">
         <v>8846993</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -1362,27 +1475,37 @@
         <v>3800</v>
       </c>
       <c r="J10">
+        <f t="shared" ref="J10:J18" si="7">2500*4</f>
+        <v>10000</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10">
         <v>25.3</v>
       </c>
-      <c r="K10" s="1">
+      <c r="N10" s="1">
         <v>11260092</v>
       </c>
-      <c r="L10" s="1">
+      <c r="O10" s="1">
         <v>8785893</v>
       </c>
-      <c r="M10" s="1">
-        <f>AVERAGE(L10:L14)</f>
+      <c r="P10" s="1">
+        <f>AVERAGE(O10:O14)</f>
         <v>9324645.5999999996</v>
       </c>
-      <c r="N10" t="s">
+      <c r="Q10" t="s">
         <v>9</v>
       </c>
-      <c r="O10">
-        <f>M10-M5</f>
+      <c r="R10">
+        <f>P10-P5</f>
         <v>976046.79999999981</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -1412,16 +1535,26 @@
         <v>3635</v>
       </c>
       <c r="J11">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11">
         <v>25</v>
       </c>
-      <c r="K11" s="1">
+      <c r="N11" s="1">
         <v>11569899</v>
       </c>
-      <c r="L11" s="1">
+      <c r="O11" s="1">
         <v>9036822</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -1451,24 +1584,34 @@
         <v>3610</v>
       </c>
       <c r="J12">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12">
         <v>25.7</v>
       </c>
-      <c r="K12" s="1">
+      <c r="N12" s="1">
         <v>12096895</v>
       </c>
-      <c r="L12" s="1">
+      <c r="O12" s="1">
         <v>9457394</v>
       </c>
-      <c r="P12" s="1">
-        <f t="shared" ref="P12" si="5">AVERAGE(L12:L16)</f>
+      <c r="S12" s="1">
+        <f t="shared" ref="S12" si="8">AVERAGE(O12:O16)</f>
         <v>9592123.4000000004</v>
       </c>
-      <c r="Q12">
-        <f t="shared" ref="Q12" si="6">P12-P7</f>
+      <c r="T12">
+        <f t="shared" ref="T12" si="9">S12-S7</f>
         <v>760584.80000000075</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -1498,23 +1641,33 @@
         <v>3765</v>
       </c>
       <c r="J13">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13">
         <v>26.1</v>
       </c>
-      <c r="K13" s="1">
+      <c r="N13" s="1">
         <v>12371672</v>
       </c>
-      <c r="L13" s="1">
+      <c r="O13" s="1">
         <v>9647032</v>
       </c>
-      <c r="M13" s="1">
-        <f>AVERAGE(L13:L17)</f>
+      <c r="P13" s="1">
+        <f>AVERAGE(O13:O17)</f>
         <v>9596499.1999999993</v>
       </c>
-      <c r="N13" t="s">
+      <c r="Q13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1982</v>
       </c>
@@ -1544,16 +1697,26 @@
         <v>4020</v>
       </c>
       <c r="J14">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14">
         <v>26.6</v>
       </c>
-      <c r="K14" s="1">
+      <c r="N14" s="1">
         <v>12425780</v>
       </c>
-      <c r="L14" s="1">
+      <c r="O14" s="1">
         <v>9696087</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1983</v>
       </c>
@@ -1583,16 +1746,26 @@
         <v>4250</v>
       </c>
       <c r="J15">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15">
         <v>26.2</v>
       </c>
-      <c r="K15" s="1">
+      <c r="N15" s="1">
         <v>12464661</v>
       </c>
-      <c r="L15" s="1">
+      <c r="O15" s="1">
         <v>9682734</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1984</v>
       </c>
@@ -1622,16 +1795,26 @@
         <v>4555</v>
       </c>
       <c r="J16">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16">
         <v>27.1</v>
       </c>
-      <c r="K16" s="1">
+      <c r="N16" s="1">
         <v>12241940</v>
       </c>
-      <c r="L16" s="1">
+      <c r="O16" s="1">
         <v>9477370</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1985</v>
       </c>
@@ -1661,24 +1844,34 @@
         <v>4864</v>
       </c>
       <c r="J17">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17">
         <v>27.8</v>
       </c>
-      <c r="K17" s="1">
+      <c r="N17" s="1">
         <v>12247055</v>
       </c>
-      <c r="L17" s="1">
+      <c r="O17" s="1">
         <v>9479273</v>
       </c>
-      <c r="P17" s="1">
-        <f t="shared" ref="P17" si="7">AVERAGE(L17:L21)</f>
+      <c r="S17" s="1">
+        <f t="shared" ref="S17" si="10">AVERAGE(O17:O21)</f>
         <v>9981154.1999999993</v>
       </c>
-      <c r="Q17">
-        <f t="shared" ref="Q17" si="8">P17-P12</f>
+      <c r="T17">
+        <f t="shared" ref="T17" si="11">S17-S12</f>
         <v>389030.79999999888</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1986</v>
       </c>
@@ -1708,27 +1901,37 @@
         <v>5044</v>
       </c>
       <c r="J18">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18">
         <v>27.9</v>
       </c>
-      <c r="K18" s="1">
+      <c r="N18" s="1">
         <v>12503511</v>
       </c>
-      <c r="L18" s="1">
+      <c r="O18" s="1">
         <v>9713893</v>
       </c>
-      <c r="M18" s="1">
-        <f>AVERAGE(L18:L22)</f>
+      <c r="P18" s="1">
+        <f>AVERAGE(O18:O22)</f>
         <v>10254243</v>
       </c>
-      <c r="N18" t="s">
+      <c r="Q18" t="s">
         <v>10</v>
       </c>
-      <c r="O18">
-        <f>M18-M13</f>
+      <c r="R18">
+        <f>P18-P13</f>
         <v>657743.80000000075</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1987</v>
       </c>
@@ -1758,16 +1961,26 @@
         <v>5149</v>
       </c>
       <c r="J19">
+        <f>2625*2+8000</f>
+        <v>13250</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19">
         <v>29.6</v>
       </c>
-      <c r="K19" s="1">
+      <c r="N19" s="1">
         <v>12766642</v>
       </c>
-      <c r="L19" s="1">
+      <c r="O19" s="1">
         <v>9973254</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1988</v>
       </c>
@@ -1797,16 +2010,26 @@
         <v>5321</v>
       </c>
       <c r="J20">
+        <f t="shared" ref="J20:J24" si="12">2625*2+8000</f>
+        <v>13250</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20">
         <v>30.3</v>
       </c>
-      <c r="K20" s="1">
+      <c r="N20" s="1">
         <v>13055337</v>
       </c>
-      <c r="L20" s="1">
+      <c r="O20" s="1">
         <v>10161388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1989</v>
       </c>
@@ -1836,16 +2059,26 @@
         <v>5426</v>
       </c>
       <c r="J21">
+        <f t="shared" si="12"/>
+        <v>13250</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21">
         <v>30.9</v>
       </c>
-      <c r="K21" s="1">
+      <c r="N21" s="1">
         <v>13538560</v>
       </c>
-      <c r="L21" s="1">
+      <c r="O21" s="1">
         <v>10577963</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1990</v>
       </c>
@@ -1878,24 +2111,34 @@
         <v>794</v>
       </c>
       <c r="J22">
+        <f t="shared" si="12"/>
+        <v>13250</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22">
         <v>32</v>
       </c>
-      <c r="K22" s="1">
+      <c r="N22" s="1">
         <v>13818637</v>
       </c>
-      <c r="L22" s="1">
+      <c r="O22" s="1">
         <v>10844717</v>
       </c>
-      <c r="P22" s="1">
-        <f t="shared" ref="P22" si="9">AVERAGE(L22:L26)</f>
+      <c r="S22" s="1">
+        <f t="shared" ref="S22" si="13">AVERAGE(O22:O26)</f>
         <v>11172323</v>
       </c>
-      <c r="Q22">
-        <f t="shared" ref="Q22" si="10">P22-P17</f>
+      <c r="T22">
+        <f t="shared" ref="T22" si="14">S22-S17</f>
         <v>1191168.8000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1991</v>
       </c>
@@ -1928,16 +2171,26 @@
         <v>51882</v>
       </c>
       <c r="J23">
+        <f t="shared" si="12"/>
+        <v>13250</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23">
         <v>33.299999999999997</v>
       </c>
-      <c r="K23" s="1">
+      <c r="N23" s="1">
         <v>14358953</v>
       </c>
-      <c r="L23" s="1">
+      <c r="O23" s="1">
         <v>11309563</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1992</v>
       </c>
@@ -1970,16 +2223,26 @@
         <v>44290</v>
       </c>
       <c r="J24">
+        <f t="shared" si="12"/>
+        <v>13250</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24">
         <v>34.4</v>
       </c>
-      <c r="K24" s="1">
+      <c r="N24" s="1">
         <v>14487359</v>
       </c>
-      <c r="L24" s="1">
+      <c r="O24" s="1">
         <v>11384567</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1993</v>
       </c>
@@ -2012,16 +2275,26 @@
         <v>35818</v>
       </c>
       <c r="J25">
+        <f>2625+3500+5500+5500</f>
+        <v>17125</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>26</v>
+      </c>
+      <c r="M25">
         <v>34</v>
       </c>
-      <c r="K25" s="1">
+      <c r="N25" s="1">
         <v>14304803</v>
       </c>
-      <c r="L25" s="1">
+      <c r="O25" s="1">
         <v>11189088</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1994</v>
       </c>
@@ -2054,16 +2327,26 @@
         <v>42843</v>
       </c>
       <c r="J26">
+        <f t="shared" ref="J26:J38" si="15">2625+3500+5500+5500</f>
+        <v>17125</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26">
         <v>34.6</v>
       </c>
-      <c r="K26" s="1">
+      <c r="N26" s="1">
         <v>14278790</v>
       </c>
-      <c r="L26" s="1">
+      <c r="O26" s="1">
         <v>11133680</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1995</v>
       </c>
@@ -2096,24 +2379,34 @@
         <v>51832</v>
       </c>
       <c r="J27">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
+        <v>26</v>
+      </c>
+      <c r="M27">
         <v>34.299999999999997</v>
       </c>
-      <c r="K27" s="1">
+      <c r="N27" s="1">
         <v>14261781</v>
       </c>
-      <c r="L27" s="1">
+      <c r="O27" s="1">
         <v>11092374</v>
       </c>
-      <c r="P27" s="1">
-        <f t="shared" ref="P27" si="11">AVERAGE(L27:L31)</f>
+      <c r="S27" s="1">
+        <f t="shared" ref="S27" si="16">AVERAGE(O27:O31)</f>
         <v>11184500</v>
       </c>
-      <c r="Q27">
-        <f t="shared" ref="Q27" si="12">P27-P22</f>
+      <c r="T27">
+        <f t="shared" ref="T27" si="17">S27-S22</f>
         <v>12177</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1996</v>
       </c>
@@ -2146,16 +2439,26 @@
         <v>58327</v>
       </c>
       <c r="J28">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28" t="s">
+        <v>26</v>
+      </c>
+      <c r="M28">
         <v>35.5</v>
       </c>
-      <c r="K28" s="1">
+      <c r="N28" s="1">
         <v>14367520</v>
       </c>
-      <c r="L28" s="1">
+      <c r="O28" s="1">
         <v>11120499</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1997</v>
       </c>
@@ -2188,16 +2491,26 @@
         <v>80547</v>
       </c>
       <c r="J29">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>26</v>
+      </c>
+      <c r="M29">
         <v>36.799999999999997</v>
       </c>
-      <c r="K29" s="1">
+      <c r="N29" s="1">
         <v>14502334</v>
       </c>
-      <c r="L29" s="1">
+      <c r="O29" s="1">
         <v>11196119</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1998</v>
       </c>
@@ -2230,16 +2543,26 @@
         <v>91360</v>
       </c>
       <c r="J30">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
+        <v>26</v>
+      </c>
+      <c r="M30">
         <v>36.5</v>
       </c>
-      <c r="K30" s="1">
+      <c r="N30" s="1">
         <v>14506967</v>
       </c>
-      <c r="L30" s="1">
+      <c r="O30" s="1">
         <v>11137769</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1999</v>
       </c>
@@ -2272,16 +2595,26 @@
         <v>116513</v>
       </c>
       <c r="J31">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>26</v>
+      </c>
+      <c r="M31">
         <v>35.6</v>
       </c>
-      <c r="K31" s="1">
+      <c r="N31" s="1">
         <v>14849691</v>
       </c>
-      <c r="L31" s="1">
+      <c r="O31" s="1">
         <v>11375739</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -2314,24 +2647,34 @@
         <v>133290</v>
       </c>
       <c r="J32">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32" t="s">
+        <v>26</v>
+      </c>
+      <c r="M32">
         <v>35.5</v>
       </c>
-      <c r="K32" s="1">
+      <c r="N32" s="1">
         <v>15312289</v>
       </c>
-      <c r="L32" s="1">
+      <c r="O32" s="1">
         <v>11752786</v>
       </c>
-      <c r="P32" s="1">
-        <f t="shared" ref="P32" si="13">AVERAGE(L32:L36)</f>
+      <c r="S32" s="1">
+        <f t="shared" ref="S32" si="18">AVERAGE(O32:O36)</f>
         <v>12515349</v>
       </c>
-      <c r="Q32">
-        <f t="shared" ref="Q32" si="14">P32-P27</f>
+      <c r="T32">
+        <f t="shared" ref="T32" si="19">S32-S27</f>
         <v>1330849</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -2364,16 +2707,26 @@
         <v>161643</v>
       </c>
       <c r="J33">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>26</v>
+      </c>
+      <c r="M33">
         <v>36.299999999999997</v>
       </c>
-      <c r="K33" s="1">
+      <c r="N33" s="1">
         <v>15927987</v>
       </c>
-      <c r="L33" s="1">
+      <c r="O33" s="1">
         <v>12233156</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2002</v>
       </c>
@@ -2406,16 +2759,26 @@
         <v>118352</v>
       </c>
       <c r="J34">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
+        <v>26</v>
+      </c>
+      <c r="M34">
         <v>36.700000000000003</v>
       </c>
-      <c r="K34" s="1">
+      <c r="N34" s="1">
         <v>16611711</v>
       </c>
-      <c r="L34" s="1">
+      <c r="O34" s="1">
         <v>12751993</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2003</v>
       </c>
@@ -2448,16 +2811,26 @@
         <v>107196</v>
       </c>
       <c r="J35">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35" t="s">
+        <v>26</v>
+      </c>
+      <c r="M35">
         <v>37.799999999999997</v>
       </c>
-      <c r="K35" s="1">
+      <c r="N35" s="1">
         <v>16911481</v>
       </c>
-      <c r="L35" s="1">
+      <c r="O35" s="1">
         <v>12858698</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2004</v>
       </c>
@@ -2490,16 +2863,26 @@
         <v>139037</v>
       </c>
       <c r="J36">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
+        <v>26</v>
+      </c>
+      <c r="M36">
         <v>38</v>
       </c>
-      <c r="K36" s="1">
+      <c r="N36" s="1">
         <v>17272044</v>
       </c>
-      <c r="L36" s="1">
+      <c r="O36" s="1">
         <v>12980112</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2005</v>
       </c>
@@ -2532,24 +2915,34 @@
         <v>124374</v>
       </c>
       <c r="J37">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37" t="s">
+        <v>26</v>
+      </c>
+      <c r="M37">
         <v>38.9</v>
       </c>
-      <c r="K37" s="1">
+      <c r="N37" s="1">
         <v>17487475</v>
       </c>
-      <c r="L37" s="1">
+      <c r="O37" s="1">
         <v>13021834</v>
       </c>
-      <c r="P37" s="1">
-        <f t="shared" ref="P37" si="15">AVERAGE(L37:L41)</f>
+      <c r="S37" s="1">
+        <f t="shared" ref="S37" si="20">AVERAGE(O37:O41)</f>
         <v>13695941.6</v>
       </c>
-      <c r="Q37">
-        <f t="shared" ref="Q37" si="16">P37-P32</f>
+      <c r="T37">
+        <f t="shared" ref="T37" si="21">S37-S32</f>
         <v>1180592.5999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2006</v>
       </c>
@@ -2582,16 +2975,26 @@
         <v>135861</v>
       </c>
       <c r="J38">
+        <f t="shared" si="15"/>
+        <v>17125</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38" t="s">
+        <v>26</v>
+      </c>
+      <c r="M38">
         <v>37.299999999999997</v>
       </c>
-      <c r="K38" s="1">
+      <c r="N38" s="1">
         <v>17754230</v>
       </c>
-      <c r="L38" s="1">
+      <c r="O38" s="1">
         <v>13175350</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2007</v>
       </c>
@@ -2624,16 +3027,26 @@
         <v>154692</v>
       </c>
       <c r="J39">
+        <f>3500+4500+5500+5500</f>
+        <v>19000</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M39">
         <v>38.799999999999997</v>
       </c>
-      <c r="K39" s="1">
+      <c r="N39" s="1">
         <v>18258138</v>
       </c>
-      <c r="L39" s="1">
+      <c r="O39" s="1">
         <v>13500894</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2008</v>
       </c>
@@ -2666,16 +3079,26 @@
         <v>130183</v>
       </c>
       <c r="J40">
+        <f t="shared" ref="J40:J49" si="22">3500+4500+5500+5500</f>
+        <v>19000</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M40">
         <v>39.6</v>
       </c>
-      <c r="K40" s="1">
+      <c r="N40" s="1">
         <v>19081686</v>
       </c>
-      <c r="L40" s="1">
+      <c r="O40" s="1">
         <v>13970862</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2009</v>
       </c>
@@ -2708,16 +3131,26 @@
         <v>110988</v>
       </c>
       <c r="J41">
+        <f t="shared" si="22"/>
+        <v>19000</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41" t="s">
+        <v>27</v>
+      </c>
+      <c r="M41">
         <v>41.3</v>
       </c>
-      <c r="K41" s="1">
+      <c r="N41" s="1">
         <v>20313594</v>
       </c>
-      <c r="L41" s="1">
+      <c r="O41" s="1">
         <v>14810768</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2010</v>
       </c>
@@ -2750,24 +3183,34 @@
         <v>117828</v>
       </c>
       <c r="J42">
+        <f t="shared" si="22"/>
+        <v>19000</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42" t="s">
+        <v>27</v>
+      </c>
+      <c r="M42">
         <v>41.2</v>
       </c>
-      <c r="K42" s="1">
+      <c r="N42" s="1">
         <v>21019438</v>
       </c>
-      <c r="L42" s="1">
+      <c r="O42" s="1">
         <v>15142171</v>
       </c>
-      <c r="P42" s="1">
-        <f t="shared" ref="P42" si="17">AVERAGE(L42:L46)</f>
+      <c r="S42" s="1">
+        <f t="shared" ref="S42" si="23">AVERAGE(O42:O46)</f>
         <v>14908929.800000001</v>
       </c>
-      <c r="Q42">
-        <f t="shared" ref="Q42" si="18">P42-P37</f>
+      <c r="T42">
+        <f t="shared" ref="T42" si="24">S42-S37</f>
         <v>1212988.2000000011</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -2800,16 +3243,26 @@
         <v>129552</v>
       </c>
       <c r="J43">
+        <f t="shared" si="22"/>
+        <v>19000</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43" t="s">
+        <v>27</v>
+      </c>
+      <c r="M43">
         <v>42</v>
       </c>
-      <c r="K43" s="1">
+      <c r="N43" s="1">
         <v>21010590</v>
       </c>
-      <c r="L43" s="1">
+      <c r="O43" s="1">
         <v>15116303</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2012</v>
       </c>
@@ -2842,16 +3295,26 @@
         <v>135991</v>
       </c>
       <c r="J44">
+        <f t="shared" si="22"/>
+        <v>19000</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44" t="s">
+        <v>27</v>
+      </c>
+      <c r="M44">
         <v>41</v>
       </c>
-      <c r="K44" s="1">
+      <c r="N44" s="1">
         <v>20644478</v>
       </c>
-      <c r="L44" s="1">
+      <c r="O44" s="1">
         <v>14884667</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2013</v>
       </c>
@@ -2884,16 +3347,26 @@
         <v>153794</v>
       </c>
       <c r="J45">
+        <f t="shared" si="22"/>
+        <v>19000</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45" t="s">
+        <v>27</v>
+      </c>
+      <c r="M45">
         <v>39.9</v>
       </c>
-      <c r="K45" s="1">
+      <c r="N45" s="1">
         <v>20376677</v>
       </c>
-      <c r="L45" s="1">
+      <c r="O45" s="1">
         <v>14746848</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2014</v>
       </c>
@@ -2926,16 +3399,26 @@
         <v>162239</v>
       </c>
       <c r="J46">
+        <f t="shared" si="22"/>
+        <v>19000</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46">
         <v>40</v>
       </c>
-      <c r="K46" s="1">
+      <c r="N46" s="1">
         <v>20209092</v>
       </c>
-      <c r="L46" s="1">
+      <c r="O46" s="1">
         <v>14654660</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2015</v>
       </c>
@@ -2968,24 +3451,34 @@
         <v>173799</v>
       </c>
       <c r="J47">
+        <f t="shared" si="22"/>
+        <v>19000</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47" t="s">
+        <v>27</v>
+      </c>
+      <c r="M47">
         <v>40.5</v>
       </c>
-      <c r="K47" s="1">
+      <c r="N47" s="1">
         <v>19988204</v>
       </c>
-      <c r="L47" s="1">
+      <c r="O47" s="1">
         <v>14572843</v>
       </c>
-      <c r="P47" s="1">
-        <f t="shared" ref="P47" si="19">AVERAGE(L47:L51)</f>
+      <c r="S47" s="1">
+        <f t="shared" ref="S47" si="25">AVERAGE(O47:O51)</f>
         <v>14572946</v>
       </c>
-      <c r="Q47">
-        <f t="shared" ref="Q47" si="20">P47-P42</f>
+      <c r="T47">
+        <f t="shared" ref="T47" si="26">S47-S42</f>
         <v>-335983.80000000075</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2016</v>
       </c>
@@ -3018,16 +3511,26 @@
         <v>181351</v>
       </c>
       <c r="J48">
+        <f t="shared" si="22"/>
+        <v>19000</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48" t="s">
+        <v>27</v>
+      </c>
+      <c r="M48">
         <v>41.2</v>
       </c>
-      <c r="K48" s="1">
+      <c r="N48" s="1">
         <v>19846904</v>
       </c>
-      <c r="L48" s="1">
+      <c r="O48" s="1">
         <v>14585840</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2017</v>
       </c>
@@ -3044,11 +3547,29 @@
       <c r="I49">
         <v>180440</v>
       </c>
-      <c r="K49" s="1">
+      <c r="J49">
+        <f t="shared" si="22"/>
+        <v>19000</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49" t="s">
+        <v>27</v>
+      </c>
+      <c r="N49" s="1">
         <v>19765598</v>
       </c>
-      <c r="L49">
+      <c r="O49">
         <v>14560155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2018</v>
+      </c>
+      <c r="L50" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
total federal undergraduate loans
</commit_message>
<xml_diff>
--- a/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
+++ b/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\research-dissertation-case-for-alt-ed\papers\section-127-effects\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACA265C-D02F-4A40-B766-1DBFA5B3639B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DF93AD-4DC1-4DCC-B986-C8599DB5C8B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
   <si>
     <t>Year</t>
   </si>
@@ -116,12 +116,15 @@
   <si>
     <t>E</t>
   </si>
+  <si>
+    <t>Total Federal Undergraduate Loans</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +258,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -554,7 +562,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -597,12 +605,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -640,6 +650,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="42" xr:uid="{CFF59EDB-1FE3-45F1-8894-1A0A49475676}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -956,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T50"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,12 +978,12 @@
     <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="19.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="15.85546875" customWidth="1"/>
+    <col min="4" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1004,37 +1015,40 @@
         <v>21</v>
       </c>
       <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -1067,27 +1081,27 @@
         <f>1500*4</f>
         <v>6000</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>25.7</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>8580887</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>6428134</v>
       </c>
-      <c r="S2" s="1">
-        <f>AVERAGE(O2:O6)</f>
+      <c r="T2" s="1">
+        <f>AVERAGE(P2:P6)</f>
         <v>7142218.7999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -1120,23 +1134,23 @@
         <f t="shared" ref="J3:J4" si="4">1500*4</f>
         <v>6000</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
         <v>24</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>26.2</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>8948644</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>6804309</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -1169,23 +1183,23 @@
         <f t="shared" si="4"/>
         <v>6000</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
         <v>24</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>25.5</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>9214860</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>7070635</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -1218,30 +1232,30 @@
         <f>100+1500+2500+2500</f>
         <v>6600</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>24</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>24</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>9602123</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <v>7419516</v>
       </c>
-      <c r="P5" s="1">
-        <f>AVERAGE(O5:O9)</f>
+      <c r="Q5" s="1">
+        <f>AVERAGE(P5:P9)</f>
         <v>8348598.7999999998</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -1274,23 +1288,23 @@
         <f t="shared" ref="J6:J8" si="5">100+1500+2500+2500</f>
         <v>6600</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
         <v>24</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>24.6</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>10223729</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <v>7988500</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -1323,31 +1337,31 @@
         <f t="shared" si="5"/>
         <v>6600</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
         <v>24</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>26.3</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>11184859</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <v>8834508</v>
       </c>
-      <c r="S7" s="1">
-        <f t="shared" ref="S7" si="6">AVERAGE(O7:O11)</f>
+      <c r="T7" s="1">
+        <f t="shared" ref="T7" si="6">AVERAGE(P7:P11)</f>
         <v>8831538.5999999996</v>
       </c>
-      <c r="T7">
-        <f>S7-S2</f>
+      <c r="U7">
+        <f>T7-T2</f>
         <v>1689319.7999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -1380,23 +1394,23 @@
         <f t="shared" si="5"/>
         <v>6600</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
         <v>24</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>26.7</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>11012137</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>8653477</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -1429,23 +1443,23 @@
         <f>2500*4</f>
         <v>10000</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
         <v>24</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>26.1</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O9" s="1">
         <v>11285787</v>
       </c>
-      <c r="O9" s="1">
+      <c r="P9" s="1">
         <v>8846993</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -1478,34 +1492,34 @@
         <f t="shared" ref="J10:J18" si="7">2500*4</f>
         <v>10000</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
         <v>24</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>25.3</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>11260092</v>
       </c>
-      <c r="O10" s="1">
+      <c r="P10" s="1">
         <v>8785893</v>
       </c>
-      <c r="P10" s="1">
-        <f>AVERAGE(O10:O14)</f>
+      <c r="Q10" s="1">
+        <f>AVERAGE(P10:P14)</f>
         <v>9324645.5999999996</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>9</v>
       </c>
-      <c r="R10">
-        <f>P10-P5</f>
+      <c r="S10">
+        <f>Q10-Q5</f>
         <v>976046.79999999981</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -1538,23 +1552,23 @@
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
         <v>24</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>25</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>11569899</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P11" s="1">
         <v>9036822</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -1587,31 +1601,31 @@
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
         <v>24</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>25.7</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>12096895</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P12" s="1">
         <v>9457394</v>
       </c>
-      <c r="S12" s="1">
-        <f t="shared" ref="S12" si="8">AVERAGE(O12:O16)</f>
+      <c r="T12" s="1">
+        <f t="shared" ref="T12" si="8">AVERAGE(P12:P16)</f>
         <v>9592123.4000000004</v>
       </c>
-      <c r="T12">
-        <f t="shared" ref="T12" si="9">S12-S7</f>
+      <c r="U12">
+        <f t="shared" ref="U12" si="9">T12-T7</f>
         <v>760584.80000000075</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -1644,30 +1658,30 @@
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
         <v>25</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>26.1</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>12371672</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P13" s="1">
         <v>9647032</v>
       </c>
-      <c r="P13" s="1">
-        <f>AVERAGE(O13:O17)</f>
+      <c r="Q13" s="1">
+        <f>AVERAGE(P13:P17)</f>
         <v>9596499.1999999993</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1982</v>
       </c>
@@ -1700,23 +1714,23 @@
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
         <v>25</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>26.6</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>12425780</v>
       </c>
-      <c r="O14" s="1">
+      <c r="P14" s="1">
         <v>9696087</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1983</v>
       </c>
@@ -1749,23 +1763,23 @@
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
         <v>25</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>26.2</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O15" s="1">
         <v>12464661</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <v>9682734</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1984</v>
       </c>
@@ -1798,23 +1812,23 @@
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
         <v>26</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>27.1</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O16" s="1">
         <v>12241940</v>
       </c>
-      <c r="O16" s="1">
+      <c r="P16" s="1">
         <v>9477370</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1985</v>
       </c>
@@ -1847,31 +1861,31 @@
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
         <v>26</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>27.8</v>
       </c>
-      <c r="N17" s="1">
+      <c r="O17" s="1">
         <v>12247055</v>
       </c>
-      <c r="O17" s="1">
+      <c r="P17" s="1">
         <v>9479273</v>
       </c>
-      <c r="S17" s="1">
-        <f t="shared" ref="S17" si="10">AVERAGE(O17:O21)</f>
+      <c r="T17" s="1">
+        <f t="shared" ref="T17" si="10">AVERAGE(P17:P21)</f>
         <v>9981154.1999999993</v>
       </c>
-      <c r="T17">
-        <f t="shared" ref="T17" si="11">S17-S12</f>
+      <c r="U17">
+        <f t="shared" ref="U17" si="11">T17-T12</f>
         <v>389030.79999999888</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1986</v>
       </c>
@@ -1904,34 +1918,34 @@
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
         <v>26</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>27.9</v>
       </c>
-      <c r="N18" s="1">
+      <c r="O18" s="1">
         <v>12503511</v>
       </c>
-      <c r="O18" s="1">
+      <c r="P18" s="1">
         <v>9713893</v>
       </c>
-      <c r="P18" s="1">
-        <f>AVERAGE(O18:O22)</f>
+      <c r="Q18" s="1">
+        <f>AVERAGE(P18:P22)</f>
         <v>10254243</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>10</v>
       </c>
-      <c r="R18">
-        <f>P18-P13</f>
+      <c r="S18">
+        <f>Q18-Q13</f>
         <v>657743.80000000075</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1987</v>
       </c>
@@ -1964,23 +1978,23 @@
         <f>2625*2+8000</f>
         <v>13250</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19" t="s">
         <v>26</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>29.6</v>
       </c>
-      <c r="N19" s="1">
+      <c r="O19" s="1">
         <v>12766642</v>
       </c>
-      <c r="O19" s="1">
+      <c r="P19" s="1">
         <v>9973254</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1988</v>
       </c>
@@ -2013,23 +2027,23 @@
         <f t="shared" ref="J20:J24" si="12">2625*2+8000</f>
         <v>13250</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20" t="s">
         <v>26</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>30.3</v>
       </c>
-      <c r="N20" s="1">
+      <c r="O20" s="1">
         <v>13055337</v>
       </c>
-      <c r="O20" s="1">
+      <c r="P20" s="1">
         <v>10161388</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1989</v>
       </c>
@@ -2062,23 +2076,23 @@
         <f t="shared" si="12"/>
         <v>13250</v>
       </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
         <v>26</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>30.9</v>
       </c>
-      <c r="N21" s="1">
+      <c r="O21" s="1">
         <v>13538560</v>
       </c>
-      <c r="O21" s="1">
+      <c r="P21" s="1">
         <v>10577963</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1990</v>
       </c>
@@ -2114,31 +2128,34 @@
         <f t="shared" si="12"/>
         <v>13250</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="K22" s="2">
+        <v>7721.4851683475999</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22" t="s">
         <v>26</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>32</v>
       </c>
-      <c r="N22" s="1">
+      <c r="O22" s="1">
         <v>13818637</v>
       </c>
-      <c r="O22" s="1">
+      <c r="P22" s="1">
         <v>10844717</v>
       </c>
-      <c r="S22" s="1">
-        <f t="shared" ref="S22" si="13">AVERAGE(O22:O26)</f>
+      <c r="T22" s="1">
+        <f t="shared" ref="T22" si="13">AVERAGE(P22:P26)</f>
         <v>11172323</v>
       </c>
-      <c r="T22">
-        <f t="shared" ref="T22" si="14">S22-S17</f>
+      <c r="U22">
+        <f t="shared" ref="U22" si="14">T22-T17</f>
         <v>1191168.8000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1991</v>
       </c>
@@ -2174,23 +2191,26 @@
         <f t="shared" si="12"/>
         <v>13250</v>
       </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="K23" s="2">
+        <v>8395.8777711599105</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23" t="s">
         <v>26</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>33.299999999999997</v>
       </c>
-      <c r="N23" s="1">
+      <c r="O23" s="1">
         <v>14358953</v>
       </c>
-      <c r="O23" s="1">
+      <c r="P23" s="1">
         <v>11309563</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1992</v>
       </c>
@@ -2226,23 +2246,26 @@
         <f t="shared" si="12"/>
         <v>13250</v>
       </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="K24" s="2">
+        <v>8734.8511773709688</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24" t="s">
         <v>26</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>34.4</v>
       </c>
-      <c r="N24" s="1">
+      <c r="O24" s="1">
         <v>14487359</v>
       </c>
-      <c r="O24" s="1">
+      <c r="P24" s="1">
         <v>11384567</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1993</v>
       </c>
@@ -2278,23 +2301,26 @@
         <f>2625+3500+5500+5500</f>
         <v>17125</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="2">
+        <v>11776.43353729859</v>
+      </c>
+      <c r="L25">
         <v>1</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>26</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>34</v>
       </c>
-      <c r="N25" s="1">
+      <c r="O25" s="1">
         <v>14304803</v>
       </c>
-      <c r="O25" s="1">
+      <c r="P25" s="1">
         <v>11189088</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1994</v>
       </c>
@@ -2330,23 +2356,26 @@
         <f t="shared" ref="J26:J38" si="15">2625+3500+5500+5500</f>
         <v>17125</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="2">
+        <v>15593.929353736819</v>
+      </c>
+      <c r="L26">
         <v>1</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>26</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>34.6</v>
       </c>
-      <c r="N26" s="1">
+      <c r="O26" s="1">
         <v>14278790</v>
       </c>
-      <c r="O26" s="1">
+      <c r="P26" s="1">
         <v>11133680</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1995</v>
       </c>
@@ -2382,31 +2411,34 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="2">
+        <v>18104.599209</v>
+      </c>
+      <c r="L27">
         <v>1</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>26</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>34.299999999999997</v>
       </c>
-      <c r="N27" s="1">
+      <c r="O27" s="1">
         <v>14261781</v>
       </c>
-      <c r="O27" s="1">
+      <c r="P27" s="1">
         <v>11092374</v>
       </c>
-      <c r="S27" s="1">
-        <f t="shared" ref="S27" si="16">AVERAGE(O27:O31)</f>
+      <c r="T27" s="1">
+        <f t="shared" ref="T27" si="16">AVERAGE(P27:P31)</f>
         <v>11184500</v>
       </c>
-      <c r="T27">
-        <f t="shared" ref="T27" si="17">S27-S22</f>
+      <c r="U27">
+        <f t="shared" ref="U27" si="17">T27-T22</f>
         <v>12177</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1996</v>
       </c>
@@ -2442,23 +2474,26 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="2">
+        <v>19946.724761000001</v>
+      </c>
+      <c r="L28">
         <v>1</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>26</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>35.5</v>
       </c>
-      <c r="N28" s="1">
+      <c r="O28" s="1">
         <v>14367520</v>
       </c>
-      <c r="O28" s="1">
+      <c r="P28" s="1">
         <v>11120499</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1997</v>
       </c>
@@ -2494,23 +2529,26 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="2">
+        <v>21085.003477999999</v>
+      </c>
+      <c r="L29">
         <v>1</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>26</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>36.799999999999997</v>
       </c>
-      <c r="N29" s="1">
+      <c r="O29" s="1">
         <v>14502334</v>
       </c>
-      <c r="O29" s="1">
+      <c r="P29" s="1">
         <v>11196119</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1998</v>
       </c>
@@ -2546,23 +2584,26 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="2">
+        <v>21712.867800000004</v>
+      </c>
+      <c r="L30">
         <v>1</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>26</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>36.5</v>
       </c>
-      <c r="N30" s="1">
+      <c r="O30" s="1">
         <v>14506967</v>
       </c>
-      <c r="O30" s="1">
+      <c r="P30" s="1">
         <v>11137769</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1999</v>
       </c>
@@ -2598,23 +2639,26 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="2">
+        <v>22583.737441000001</v>
+      </c>
+      <c r="L31">
         <v>1</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>26</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>35.6</v>
       </c>
-      <c r="N31" s="1">
+      <c r="O31" s="1">
         <v>14849691</v>
       </c>
-      <c r="O31" s="1">
+      <c r="P31" s="1">
         <v>11375739</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -2650,31 +2694,34 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="2">
+        <v>23694.724191000001</v>
+      </c>
+      <c r="L32">
         <v>1</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>26</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>35.5</v>
       </c>
-      <c r="N32" s="1">
+      <c r="O32" s="1">
         <v>15312289</v>
       </c>
-      <c r="O32" s="1">
+      <c r="P32" s="1">
         <v>11752786</v>
       </c>
-      <c r="S32" s="1">
-        <f t="shared" ref="S32" si="18">AVERAGE(O32:O36)</f>
+      <c r="T32" s="1">
+        <f t="shared" ref="T32" si="18">AVERAGE(P32:P36)</f>
         <v>12515349</v>
       </c>
-      <c r="T32">
-        <f t="shared" ref="T32" si="19">S32-S27</f>
+      <c r="U32">
+        <f t="shared" ref="U32" si="19">T32-T27</f>
         <v>1330849</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -2710,23 +2757,26 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="2">
+        <v>25858.497605</v>
+      </c>
+      <c r="L33">
         <v>1</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>26</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>36.299999999999997</v>
       </c>
-      <c r="N33" s="1">
+      <c r="O33" s="1">
         <v>15927987</v>
       </c>
-      <c r="O33" s="1">
+      <c r="P33" s="1">
         <v>12233156</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2002</v>
       </c>
@@ -2762,23 +2812,26 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="2">
+        <v>29237.889558000003</v>
+      </c>
+      <c r="L34">
         <v>1</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>26</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>36.700000000000003</v>
       </c>
-      <c r="N34" s="1">
+      <c r="O34" s="1">
         <v>16611711</v>
       </c>
-      <c r="O34" s="1">
+      <c r="P34" s="1">
         <v>12751993</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2003</v>
       </c>
@@ -2814,23 +2867,26 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="2">
+        <v>33729.110334000005</v>
+      </c>
+      <c r="L35">
         <v>1</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>26</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <v>37.799999999999997</v>
       </c>
-      <c r="N35" s="1">
+      <c r="O35" s="1">
         <v>16911481</v>
       </c>
-      <c r="O35" s="1">
+      <c r="P35" s="1">
         <v>12858698</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2004</v>
       </c>
@@ -2866,23 +2922,26 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="2">
+        <v>37174.845230999999</v>
+      </c>
+      <c r="L36">
         <v>1</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>26</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>38</v>
       </c>
-      <c r="N36" s="1">
+      <c r="O36" s="1">
         <v>17272044</v>
       </c>
-      <c r="O36" s="1">
+      <c r="P36" s="1">
         <v>12980112</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2005</v>
       </c>
@@ -2918,31 +2977,34 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="2">
+        <v>39261.861787000002</v>
+      </c>
+      <c r="L37">
         <v>1</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>26</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>38.9</v>
       </c>
-      <c r="N37" s="1">
+      <c r="O37" s="1">
         <v>17487475</v>
       </c>
-      <c r="O37" s="1">
+      <c r="P37" s="1">
         <v>13021834</v>
       </c>
-      <c r="S37" s="1">
-        <f t="shared" ref="S37" si="20">AVERAGE(O37:O41)</f>
+      <c r="T37" s="1">
+        <f t="shared" ref="T37" si="20">AVERAGE(P37:P41)</f>
         <v>13695941.6</v>
       </c>
-      <c r="T37">
-        <f t="shared" ref="T37" si="21">S37-S32</f>
+      <c r="U37">
+        <f t="shared" ref="U37" si="21">T37-T32</f>
         <v>1180592.5999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2006</v>
       </c>
@@ -2978,23 +3040,26 @@
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="2">
+        <v>39865.693807000003</v>
+      </c>
+      <c r="L38">
         <v>1</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>26</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>37.299999999999997</v>
       </c>
-      <c r="N38" s="1">
+      <c r="O38" s="1">
         <v>17754230</v>
       </c>
-      <c r="O38" s="1">
+      <c r="P38" s="1">
         <v>13175350</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2007</v>
       </c>
@@ -3030,23 +3095,26 @@
         <f>3500+4500+5500+5500</f>
         <v>19000</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="2">
+        <v>43820.560598000004</v>
+      </c>
+      <c r="L39">
         <v>1</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>26</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>38.799999999999997</v>
       </c>
-      <c r="N39" s="1">
+      <c r="O39" s="1">
         <v>18258138</v>
       </c>
-      <c r="O39" s="1">
+      <c r="P39" s="1">
         <v>13500894</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2008</v>
       </c>
@@ -3082,23 +3150,26 @@
         <f t="shared" ref="J40:J49" si="22">3500+4500+5500+5500</f>
         <v>19000</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="2">
+        <v>57913.02765051715</v>
+      </c>
+      <c r="L40">
         <v>1</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>26</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <v>39.6</v>
       </c>
-      <c r="N40" s="1">
+      <c r="O40" s="1">
         <v>19081686</v>
       </c>
-      <c r="O40" s="1">
+      <c r="P40" s="1">
         <v>13970862</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2009</v>
       </c>
@@ -3134,23 +3205,26 @@
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="2">
+        <v>67681.483983686572</v>
+      </c>
+      <c r="L41">
         <v>1</v>
       </c>
-      <c r="L41" t="s">
+      <c r="M41" t="s">
         <v>27</v>
       </c>
-      <c r="M41">
+      <c r="N41">
         <v>41.3</v>
       </c>
-      <c r="N41" s="1">
+      <c r="O41" s="1">
         <v>20313594</v>
       </c>
-      <c r="O41" s="1">
+      <c r="P41" s="1">
         <v>14810768</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2010</v>
       </c>
@@ -3186,31 +3260,34 @@
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="2">
+        <v>70899.286510563674</v>
+      </c>
+      <c r="L42">
         <v>1</v>
       </c>
-      <c r="L42" t="s">
+      <c r="M42" t="s">
         <v>27</v>
       </c>
-      <c r="M42">
+      <c r="N42">
         <v>41.2</v>
       </c>
-      <c r="N42" s="1">
+      <c r="O42" s="1">
         <v>21019438</v>
       </c>
-      <c r="O42" s="1">
+      <c r="P42" s="1">
         <v>15142171</v>
       </c>
-      <c r="S42" s="1">
-        <f t="shared" ref="S42" si="23">AVERAGE(O42:O46)</f>
+      <c r="T42" s="1">
+        <f t="shared" ref="T42" si="23">AVERAGE(P42:P46)</f>
         <v>14908929.800000001</v>
       </c>
-      <c r="T42">
-        <f t="shared" ref="T42" si="24">S42-S37</f>
+      <c r="U42">
+        <f t="shared" ref="U42" si="24">T42-T37</f>
         <v>1212988.2000000011</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -3246,23 +3323,26 @@
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="2">
+        <v>71294.597505559141</v>
+      </c>
+      <c r="L43">
         <v>1</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
         <v>27</v>
       </c>
-      <c r="M43">
+      <c r="N43">
         <v>42</v>
       </c>
-      <c r="N43" s="1">
+      <c r="O43" s="1">
         <v>21010590</v>
       </c>
-      <c r="O43" s="1">
+      <c r="P43" s="1">
         <v>15116303</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2012</v>
       </c>
@@ -3298,23 +3378,26 @@
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="2">
+        <v>67937.063653967853</v>
+      </c>
+      <c r="L44">
         <v>1</v>
       </c>
-      <c r="L44" t="s">
+      <c r="M44" t="s">
         <v>27</v>
       </c>
-      <c r="M44">
+      <c r="N44">
         <v>41</v>
       </c>
-      <c r="N44" s="1">
+      <c r="O44" s="1">
         <v>20644478</v>
       </c>
-      <c r="O44" s="1">
+      <c r="P44" s="1">
         <v>14884667</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2013</v>
       </c>
@@ -3350,23 +3433,26 @@
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="2">
+        <v>65652.303782821924</v>
+      </c>
+      <c r="L45">
         <v>1</v>
       </c>
-      <c r="L45" t="s">
+      <c r="M45" t="s">
         <v>27</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <v>39.9</v>
       </c>
-      <c r="N45" s="1">
+      <c r="O45" s="1">
         <v>20376677</v>
       </c>
-      <c r="O45" s="1">
+      <c r="P45" s="1">
         <v>14746848</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2014</v>
       </c>
@@ -3402,23 +3488,26 @@
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K46">
+      <c r="K46" s="2">
+        <v>62423.127847651929</v>
+      </c>
+      <c r="L46">
         <v>1</v>
       </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
         <v>27</v>
       </c>
-      <c r="M46">
+      <c r="N46">
         <v>40</v>
       </c>
-      <c r="N46" s="1">
+      <c r="O46" s="1">
         <v>20209092</v>
       </c>
-      <c r="O46" s="1">
+      <c r="P46" s="1">
         <v>14654660</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2015</v>
       </c>
@@ -3454,31 +3543,34 @@
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="2">
+        <v>59815.726707200003</v>
+      </c>
+      <c r="L47">
         <v>1</v>
       </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
         <v>27</v>
       </c>
-      <c r="M47">
+      <c r="N47">
         <v>40.5</v>
       </c>
-      <c r="N47" s="1">
+      <c r="O47" s="1">
         <v>19988204</v>
       </c>
-      <c r="O47" s="1">
+      <c r="P47" s="1">
         <v>14572843</v>
       </c>
-      <c r="S47" s="1">
-        <f t="shared" ref="S47" si="25">AVERAGE(O47:O51)</f>
+      <c r="T47" s="1">
+        <f t="shared" ref="T47" si="25">AVERAGE(P47:P51)</f>
         <v>14572946</v>
       </c>
-      <c r="T47">
-        <f t="shared" ref="T47" si="26">S47-S42</f>
+      <c r="U47">
+        <f t="shared" ref="U47" si="26">T47-T42</f>
         <v>-335983.80000000075</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2016</v>
       </c>
@@ -3514,23 +3606,26 @@
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="2">
+        <v>57805.074495200002</v>
+      </c>
+      <c r="L48">
         <v>1</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M48" t="s">
         <v>27</v>
       </c>
-      <c r="M48">
+      <c r="N48">
         <v>41.2</v>
       </c>
-      <c r="N48" s="1">
+      <c r="O48" s="1">
         <v>19846904</v>
       </c>
-      <c r="O48" s="1">
+      <c r="P48" s="1">
         <v>14585840</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2017</v>
       </c>
@@ -3551,24 +3646,61 @@
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="2">
+        <v>55808.355549400003</v>
+      </c>
+      <c r="L49">
         <v>1</v>
       </c>
-      <c r="L49" t="s">
+      <c r="M49" t="s">
         <v>27</v>
       </c>
-      <c r="N49" s="1">
+      <c r="O49" s="1">
         <v>19765598</v>
       </c>
-      <c r="O49">
+      <c r="P49">
         <v>14560155</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2018</v>
       </c>
-      <c r="L50" t="s">
+      <c r="B50">
+        <v>5250</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2019</v>
+      </c>
+      <c r="B51">
+        <v>5250</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2020</v>
+      </c>
+      <c r="B52">
+        <v>5250</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
section 127 takes effect 1979 not 1978
</commit_message>
<xml_diff>
--- a/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
+++ b/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\research-dissertation-case-for-alt-ed\papers\section-127-effects\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DE9BE8-C3B0-4A9E-B330-F6852F10B7DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84B3179-8797-4FF8-9B7E-AE5094D0D7F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,23 +1464,23 @@
         <v>1978</v>
       </c>
       <c r="B10">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>44818.011366965482</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>144113.49497182926</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>11.794213517622495</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>37.92460393995507</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1422.25</v>

</xml_diff>

<commit_message>
1981 record fix and explicit deflator variables
explicit deflator variables enable simpler real price formula
and easier communication and reference from the paper
</commit_message>
<xml_diff>
--- a/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
+++ b/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\research-dissertation-case-for-alt-ed\papers\section-127-effects\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84B3179-8797-4FF8-9B7E-AE5094D0D7F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC39CF10-DB84-46CE-8B50-6A30C1DCAFCA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="section-127-effects" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Unused_5 Year Growth Delta</t>
+  </si>
+  <si>
+    <t>2016-Based PCE Deflator</t>
+  </si>
+  <si>
+    <t>2016-Based Education-Specific Deflator</t>
   </si>
 </sst>
 </file>
@@ -967,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U52"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,12 +984,12 @@
     <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="15.85546875" customWidth="1"/>
+    <col min="4" max="15" width="19.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1009,46 +1015,52 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>25</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>28</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -1056,19 +1068,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C47" si="0">B2*($G$48/G2)</f>
+        <f>B2/I2</f>
         <v>0</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D47" si="1">C2*($H$48/H2)</f>
+        <f>C2/J2</f>
         <v>0</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E47" si="2">C2/H2</f>
+        <f>C2/H2</f>
         <v>0</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F47" si="3">D2/H2</f>
+        <f t="shared" ref="F2:F47" si="0">D2/H2</f>
         <v>0</v>
       </c>
       <c r="G2">
@@ -1077,31 +1089,39 @@
       <c r="H2">
         <v>4203</v>
       </c>
+      <c r="I2">
+        <f>G2/$G$48</f>
+        <v>5.0729563908909432E-2</v>
+      </c>
       <c r="J2">
+        <f>H2/$H$48</f>
+        <v>0.34397250184139455</v>
+      </c>
+      <c r="L2">
         <f>1500*4</f>
         <v>6000</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
         <v>19</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>25.7</v>
       </c>
-      <c r="O2" s="1">
+      <c r="Q2" s="1">
         <v>8580887</v>
       </c>
-      <c r="P2" s="1">
+      <c r="R2" s="1">
         <v>6428134</v>
       </c>
-      <c r="T2" s="1">
-        <f>AVERAGE(P2:P6)</f>
+      <c r="V2" s="1">
+        <f>AVERAGE(R2:R6)</f>
         <v>7142218.7999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -1109,19 +1129,19 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C3:C49" si="1">B3/I3</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D3:D49" si="2">C3/J3</f>
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" si="2"/>
+        <f>C3/H3</f>
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G3">
@@ -1130,27 +1150,35 @@
       <c r="H3">
         <v>4268</v>
       </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I52" si="3">G3/$G$48</f>
+        <v>5.4902609329998728E-2</v>
+      </c>
       <c r="J3">
-        <f t="shared" ref="J3:J4" si="4">1500*4</f>
+        <f>H3/$H$48</f>
+        <v>0.34929208609542517</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L4" si="4">1500*4</f>
         <v>6000</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
         <v>19</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>26.2</v>
       </c>
-      <c r="O3" s="1">
+      <c r="Q3" s="1">
         <v>8948644</v>
       </c>
-      <c r="P3" s="1">
+      <c r="R3" s="1">
         <v>6804309</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -1158,19 +1186,19 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
+        <f>C4/H4</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4">
@@ -1179,27 +1207,35 @@
       <c r="H4">
         <v>4305</v>
       </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>6.0254226319732165E-2</v>
+      </c>
       <c r="J4">
+        <f>H4/$H$48</f>
+        <v>0.35232015713233489</v>
+      </c>
+      <c r="L4">
         <f t="shared" si="4"/>
         <v>6000</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
         <v>19</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>25.5</v>
       </c>
-      <c r="O4" s="1">
+      <c r="Q4" s="1">
         <v>9214860</v>
       </c>
-      <c r="P4" s="1">
+      <c r="R4" s="1">
         <v>7070635</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -1207,19 +1243,19 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f>C5/H5</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G5">
@@ -1228,34 +1264,42 @@
       <c r="H5">
         <v>4141</v>
       </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>6.6641914266925895E-2</v>
+      </c>
       <c r="J5">
+        <f>H5/$H$48</f>
+        <v>0.33889843686062687</v>
+      </c>
+      <c r="L5">
         <f>100+1500+2500+2500</f>
         <v>6600</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
         <v>19</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>24</v>
       </c>
-      <c r="O5" s="1">
+      <c r="Q5" s="1">
         <v>9602123</v>
       </c>
-      <c r="P5" s="1">
+      <c r="R5" s="1">
         <v>7419516</v>
       </c>
-      <c r="Q5" s="1">
-        <f>AVERAGE(P5:P9)</f>
+      <c r="S5" s="1">
+        <f>AVERAGE(R5:R9)</f>
         <v>8348598.7999999998</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -1263,19 +1307,19 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f>C6/H6</f>
         <v>0</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6">
@@ -1284,27 +1328,35 @@
       <c r="H6">
         <v>3792</v>
       </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>7.2961620271169522E-2</v>
+      </c>
       <c r="J6">
-        <f t="shared" ref="J6:J8" si="5">100+1500+2500+2500</f>
+        <f>H6/$H$48</f>
+        <v>0.31033636140437026</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L8" si="5">100+1500+2500+2500</f>
         <v>6600</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
         <v>19</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>24.6</v>
       </c>
-      <c r="O6" s="1">
+      <c r="Q6" s="1">
         <v>10223729</v>
       </c>
-      <c r="P6" s="1">
+      <c r="R6" s="1">
         <v>7988500</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -1312,19 +1364,19 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f>C7/H7</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7">
@@ -1333,35 +1385,43 @@
       <c r="H7">
         <v>3628</v>
       </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>8.0837720565452881E-2</v>
+      </c>
       <c r="J7">
+        <f>H7/$H$48</f>
+        <v>0.29691464113266225</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="5"/>
         <v>6600</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
         <v>19</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>26.3</v>
       </c>
-      <c r="O7" s="1">
+      <c r="Q7" s="1">
         <v>11184859</v>
       </c>
-      <c r="P7" s="1">
+      <c r="R7" s="1">
         <v>8834508</v>
       </c>
-      <c r="T7" s="1">
-        <f t="shared" ref="T7" si="6">AVERAGE(P7:P11)</f>
+      <c r="V7" s="1">
+        <f t="shared" ref="V7" si="6">AVERAGE(R7:R11)</f>
         <v>8831538.5999999996</v>
       </c>
-      <c r="U7">
-        <f>T7-T2</f>
+      <c r="W7">
+        <f>V7-V2</f>
         <v>1689319.7999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -1369,19 +1429,19 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f>C8/H8</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G8">
@@ -1390,27 +1450,35 @@
       <c r="H8">
         <v>3820</v>
       </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>9.0023780606581963E-2</v>
+      </c>
       <c r="J8">
+        <f>H8/$H$48</f>
+        <v>0.31262787462149111</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="5"/>
         <v>6600</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
         <v>19</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>26.7</v>
       </c>
-      <c r="O8" s="1">
+      <c r="Q8" s="1">
         <v>11012137</v>
       </c>
-      <c r="P8" s="1">
+      <c r="R8" s="1">
         <v>8653477</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -1418,19 +1486,19 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f>C9/H9</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G9">
@@ -1439,27 +1507,35 @@
       <c r="H9">
         <v>3814</v>
       </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>9.9931495119027255E-2</v>
+      </c>
       <c r="J9">
+        <f>H9/$H$48</f>
+        <v>0.31213683607496523</v>
+      </c>
+      <c r="L9">
         <f>2500*4</f>
         <v>10000</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
         <v>19</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>26.1</v>
       </c>
-      <c r="O9" s="1">
+      <c r="Q9" s="1">
         <v>11285787</v>
       </c>
-      <c r="P9" s="1">
+      <c r="R9" s="1">
         <v>8846993</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -1467,19 +1543,19 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f>C10/H10</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G10">
@@ -1488,38 +1564,46 @@
       <c r="H10">
         <v>3800</v>
       </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>0.1115622904162456</v>
+      </c>
       <c r="J10">
-        <f t="shared" ref="J10:J18" si="7">2500*4</f>
+        <f>H10/$H$48</f>
+        <v>0.31099107946640475</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L18" si="7">2500*4</f>
         <v>10000</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
         <v>19</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>25.3</v>
       </c>
-      <c r="O10" s="1">
+      <c r="Q10" s="1">
         <v>11260092</v>
       </c>
-      <c r="P10" s="1">
+      <c r="R10" s="1">
         <v>8785893</v>
       </c>
-      <c r="Q10" s="1">
-        <f>AVERAGE(P10:P14)</f>
+      <c r="S10" s="1">
+        <f>AVERAGE(R10:R14)</f>
         <v>9324645.5999999996</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>9</v>
       </c>
-      <c r="S10">
-        <f>Q10-Q5</f>
+      <c r="U10">
+        <f>S10-S5</f>
         <v>976046.79999999981</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -1527,20 +1611,20 @@
         <v>5000</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>40205.25516291635</v>
+        <f t="shared" si="1"/>
+        <v>40205.255162916357</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>135149.38454901648</v>
+        <f t="shared" si="2"/>
+        <v>135149.38454901651</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>11.060592892136548</v>
+        <f>C11/H11</f>
+        <v>11.060592892136549</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
-        <v>37.180023259701919</v>
+        <f t="shared" si="0"/>
+        <v>37.180023259701926</v>
       </c>
       <c r="G11">
         <v>1585.425</v>
@@ -1548,27 +1632,35 @@
       <c r="H11">
         <v>3635</v>
       </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0.12436185219418258</v>
+      </c>
       <c r="J11">
+        <f>H11/$H$48</f>
+        <v>0.29748751943694246</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
         <v>19</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>25</v>
       </c>
-      <c r="O11" s="1">
+      <c r="Q11" s="1">
         <v>11569899</v>
       </c>
-      <c r="P11" s="1">
+      <c r="R11" s="1">
         <v>9036822</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -1576,20 +1668,20 @@
         <v>5000</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>36410.367479055603</v>
+        <f t="shared" si="1"/>
+        <v>36410.367479055596</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
-        <v>123240.52083838792</v>
+        <f t="shared" si="2"/>
+        <v>123240.52083838789</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
-        <v>10.085974370929531</v>
+        <f>C12/H12</f>
+        <v>10.085974370929527</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
-        <v>34.138648431686406</v>
+        <f t="shared" si="0"/>
+        <v>34.138648431686399</v>
       </c>
       <c r="G12">
         <v>1750.6666666666663</v>
@@ -1597,35 +1689,43 @@
       <c r="H12">
         <v>3610</v>
       </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>0.13732352475915435</v>
+      </c>
       <c r="J12">
+        <f>H12/$H$48</f>
+        <v>0.29544152549308456</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
         <v>19</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>25.7</v>
       </c>
-      <c r="O12" s="1">
+      <c r="Q12" s="1">
         <v>12096895</v>
       </c>
-      <c r="P12" s="1">
+      <c r="R12" s="1">
         <v>9457394</v>
       </c>
-      <c r="T12" s="1">
-        <f t="shared" ref="T12" si="8">AVERAGE(P12:P16)</f>
+      <c r="V12" s="1">
+        <f t="shared" ref="V12" si="8">AVERAGE(R12:R16)</f>
         <v>9592123.4000000004</v>
       </c>
-      <c r="U12">
-        <f t="shared" ref="U12" si="9">T12-T7</f>
+      <c r="W12">
+        <f t="shared" ref="W12" si="9">V12-V7</f>
         <v>760584.80000000075</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -1633,55 +1733,63 @@
         <v>5000</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32959.844531677532</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>106968.4834880658</v>
+        <f t="shared" si="2"/>
+        <v>107224.79774562508</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
-        <v>8.754274776009968</v>
+        <f>C13/H13</f>
+        <v>8.7752514727575956</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
-        <v>28.411283794970995</v>
+        <f t="shared" si="0"/>
+        <v>28.547603233659501</v>
       </c>
       <c r="G13">
         <v>1933.9416666666666</v>
       </c>
       <c r="H13">
-        <v>3765</v>
+        <v>3756</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>0.15169974467551042</v>
       </c>
       <c r="J13">
+        <f>H13/$H$48</f>
+        <v>0.30739013012521482</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
         <v>20</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>26.1</v>
       </c>
-      <c r="O13" s="1">
+      <c r="Q13" s="1">
         <v>12371672</v>
       </c>
-      <c r="P13" s="1">
+      <c r="R13" s="1">
         <v>9647032</v>
       </c>
-      <c r="Q13" s="1">
-        <f>AVERAGE(P13:P17)</f>
+      <c r="S13" s="1">
+        <f>AVERAGE(R13:R17)</f>
         <v>9596499.1999999993</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1982</v>
       </c>
@@ -1689,19 +1797,19 @@
         <v>5000</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30774.977972150362</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>93542.153194454047</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f>C14/H14</f>
         <v>7.6554671572513335</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>23.269192336928867</v>
       </c>
       <c r="G14">
@@ -1710,27 +1818,35 @@
       <c r="H14">
         <v>4020</v>
       </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>0.1624696532528706</v>
+      </c>
       <c r="J14">
+        <f>H14/$H$48</f>
+        <v>0.32899582617235451</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
         <v>20</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>26.6</v>
       </c>
-      <c r="O14" s="1">
+      <c r="Q14" s="1">
         <v>12425780</v>
       </c>
-      <c r="P14" s="1">
+      <c r="R14" s="1">
         <v>9696087</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1983</v>
       </c>
@@ -1738,20 +1854,20 @@
         <v>5000</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>27937.492923485992</v>
+        <f t="shared" si="1"/>
+        <v>27937.492923485988</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>80321.935536958903</v>
+        <f t="shared" si="2"/>
+        <v>80321.935536958888</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
-        <v>6.5735277467025863</v>
+        <f>C15/H15</f>
+        <v>6.5735277467025854</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
-        <v>18.899278949872684</v>
+        <f t="shared" si="0"/>
+        <v>18.899278949872681</v>
       </c>
       <c r="G15">
         <v>2281.6083333333331</v>
@@ -1759,27 +1875,35 @@
       <c r="H15">
         <v>4250</v>
       </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>0.17897096255894493</v>
+      </c>
       <c r="J15">
+        <f>H15/$H$48</f>
+        <v>0.34781897045584748</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
         <v>20</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>26.2</v>
       </c>
-      <c r="O15" s="1">
+      <c r="Q15" s="1">
         <v>12464661</v>
       </c>
-      <c r="P15" s="1">
+      <c r="R15" s="1">
         <v>9682734</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1984</v>
       </c>
@@ -1787,20 +1911,20 @@
         <v>5000</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
-        <v>25575.397886853014</v>
+        <f t="shared" si="1"/>
+        <v>25575.39788685301</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>68607.197975731498</v>
+        <f t="shared" si="2"/>
+        <v>68607.197975731484</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
-        <v>5.6147964625363365</v>
+        <f>C16/H16</f>
+        <v>5.6147964625363356</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
-        <v>15.061953452410867</v>
+        <f t="shared" si="0"/>
+        <v>15.061953452410863</v>
       </c>
       <c r="G16">
         <v>2492.3333333333335</v>
@@ -1808,27 +1932,35 @@
       <c r="H16">
         <v>4555</v>
       </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>0.19550037978373902</v>
+      </c>
       <c r="J16">
+        <f>H16/$H$48</f>
+        <v>0.37278009657091415</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16" t="s">
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
         <v>21</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>27.1</v>
       </c>
-      <c r="O16" s="1">
+      <c r="Q16" s="1">
         <v>12241940</v>
       </c>
-      <c r="P16" s="1">
+      <c r="R16" s="1">
         <v>9477370</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1985</v>
       </c>
@@ -1836,20 +1968,20 @@
         <v>5000</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23496.548821807392</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>59026.38364590142</v>
+        <f t="shared" si="2"/>
+        <v>59026.383645901427</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f>C17/H17</f>
         <v>4.8307049386939536</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
-        <v>12.135358479831707</v>
+        <f t="shared" si="0"/>
+        <v>12.135358479831709</v>
       </c>
       <c r="G17">
         <v>2712.8416666666662</v>
@@ -1857,35 +1989,43 @@
       <c r="H17">
         <v>4864</v>
       </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>0.21279720855683487</v>
+      </c>
       <c r="J17">
+        <f>H17/$H$48</f>
+        <v>0.3980685817169981</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" t="s">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
         <v>21</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>27.8</v>
       </c>
-      <c r="O17" s="1">
+      <c r="Q17" s="1">
         <v>12247055</v>
       </c>
-      <c r="P17" s="1">
+      <c r="R17" s="1">
         <v>9479273</v>
       </c>
-      <c r="T17" s="1">
-        <f t="shared" ref="T17" si="10">AVERAGE(P17:P21)</f>
+      <c r="V17" s="1">
+        <f t="shared" ref="V17" si="10">AVERAGE(R17:R21)</f>
         <v>9981154.1999999993</v>
       </c>
-      <c r="U17">
-        <f t="shared" ref="U17" si="11">T17-T12</f>
+      <c r="W17">
+        <f t="shared" ref="W17" si="11">V17-V12</f>
         <v>389030.79999999888</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1986</v>
       </c>
@@ -1893,20 +2033,20 @@
         <v>5250</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
-        <v>23188.898320499604</v>
+        <f t="shared" si="1"/>
+        <v>23188.8983204996</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
-        <v>56174.692422320506</v>
+        <f t="shared" si="2"/>
+        <v>56174.692422320499</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
-        <v>4.5973232197659799</v>
+        <f>C18/H18</f>
+        <v>4.597323219765979</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
-        <v>11.136933469928728</v>
+        <f t="shared" si="0"/>
+        <v>11.136933469928726</v>
       </c>
       <c r="G18">
         <v>2886.2750000000001</v>
@@ -1914,38 +2054,46 @@
       <c r="H18">
         <v>5044</v>
       </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>0.22640144121719058</v>
+      </c>
       <c r="J18">
+        <f>H18/$H$48</f>
+        <v>0.41279973811277521</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18" t="s">
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
         <v>21</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>27.9</v>
       </c>
-      <c r="O18" s="1">
+      <c r="Q18" s="1">
         <v>12503511</v>
       </c>
-      <c r="P18" s="1">
+      <c r="R18" s="1">
         <v>9713893</v>
       </c>
-      <c r="Q18" s="1">
-        <f>AVERAGE(P18:P22)</f>
+      <c r="S18" s="1">
+        <f>AVERAGE(R18:R22)</f>
         <v>10254243</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>10</v>
       </c>
-      <c r="S18">
-        <f>Q18-Q13</f>
+      <c r="U18">
+        <f>S18-S13</f>
         <v>657743.80000000075</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1987</v>
       </c>
@@ -1953,19 +2101,19 @@
         <v>5250</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21756.682188685991</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51630.394185968951</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f>C19/H19</f>
         <v>4.2254189529395978</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>10.027266301411721</v>
       </c>
       <c r="G19">
@@ -1974,27 +2122,35 @@
       <c r="H19">
         <v>5149</v>
       </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>0.24130517486393807</v>
+      </c>
       <c r="J19">
+        <f>H19/$H$48</f>
+        <v>0.42139291267697848</v>
+      </c>
+      <c r="L19">
         <f>2625*2+8000</f>
         <v>13250</v>
       </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
         <v>21</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>29.6</v>
       </c>
-      <c r="O19" s="1">
+      <c r="Q19" s="1">
         <v>12766642</v>
       </c>
-      <c r="P19" s="1">
+      <c r="R19" s="1">
         <v>9973254</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1988</v>
       </c>
@@ -2002,19 +2158,19 @@
         <v>5250</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20098.960210210211</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46154.706786047471</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f>C20/H20</f>
         <v>3.7772900225916577</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>8.6740663007042791</v>
       </c>
       <c r="G20">
@@ -2023,27 +2179,35 @@
       <c r="H20">
         <v>5321</v>
       </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>0.26120754233510129</v>
+      </c>
       <c r="J20">
-        <f t="shared" ref="J20:J24" si="12">2625*2+8000</f>
+        <f>H20/$H$48</f>
+        <v>0.43546935101072098</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ref="L20:L24" si="12">2625*2+8000</f>
         <v>13250</v>
       </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20" t="s">
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
         <v>21</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <v>30.3</v>
       </c>
-      <c r="O20" s="1">
+      <c r="Q20" s="1">
         <v>13055337</v>
       </c>
-      <c r="P20" s="1">
+      <c r="R20" s="1">
         <v>10161388</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1989</v>
       </c>
@@ -2051,20 +2215,20 @@
         <v>5250</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>18712.301846173919</v>
+        <f t="shared" si="1"/>
+        <v>18712.301846173916</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
-        <v>42138.889837522875</v>
+        <f t="shared" si="2"/>
+        <v>42138.889837522867</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
-        <v>3.4486365363387246</v>
+        <f>C21/H21</f>
+        <v>3.4486365363387237</v>
       </c>
       <c r="F21">
-        <f t="shared" si="3"/>
-        <v>7.7661057570075327</v>
+        <f t="shared" si="0"/>
+        <v>7.7661057570075318</v>
       </c>
       <c r="G21">
         <v>3576.7666666666664</v>
@@ -2072,27 +2236,35 @@
       <c r="H21">
         <v>5426</v>
       </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>0.28056409324507886</v>
+      </c>
       <c r="J21">
+        <f>H21/$H$48</f>
+        <v>0.44406252557492432</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="12"/>
         <v>13250</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
         <v>21</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>30.9</v>
       </c>
-      <c r="O21" s="1">
+      <c r="Q21" s="1">
         <v>13538560</v>
       </c>
-      <c r="P21" s="1">
+      <c r="R21" s="1">
         <v>10577963</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1990</v>
       </c>
@@ -2100,19 +2272,19 @@
         <v>5250</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17571.419663953791</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39287.31507298287</v>
       </c>
       <c r="E22">
-        <f t="shared" si="2"/>
+        <f>C22/H22</f>
         <v>3.2152643483904466</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>7.1888957132631051</v>
       </c>
       <c r="G22">
@@ -2122,40 +2294,48 @@
         <v>5465</v>
       </c>
       <c r="I22">
+        <f t="shared" si="3"/>
+        <v>0.2987806392655859</v>
+      </c>
+      <c r="J22">
+        <f>H22/$H$48</f>
+        <v>0.44725427612734264</v>
+      </c>
+      <c r="K22">
         <v>794</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <f t="shared" si="12"/>
         <v>13250</v>
       </c>
-      <c r="K22" s="2">
+      <c r="M22" s="2">
         <v>7721.4851683475999</v>
       </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22" t="s">
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
         <v>21</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>32</v>
       </c>
-      <c r="O22" s="1">
+      <c r="Q22" s="1">
         <v>13818637</v>
       </c>
-      <c r="P22" s="1">
+      <c r="R22" s="1">
         <v>10844717</v>
       </c>
-      <c r="T22" s="1">
-        <f t="shared" ref="T22" si="13">AVERAGE(P22:P26)</f>
+      <c r="V22" s="1">
+        <f t="shared" ref="V22" si="13">AVERAGE(R22:R26)</f>
         <v>11172323</v>
       </c>
-      <c r="U22">
-        <f t="shared" ref="U22" si="14">T22-T17</f>
+      <c r="W22">
+        <f t="shared" ref="W22" si="14">V22-V17</f>
         <v>1191168.8000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1991</v>
       </c>
@@ -2163,19 +2343,19 @@
         <v>5250</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16972.330700275139</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35954.387799351927</v>
       </c>
       <c r="E23">
-        <f t="shared" si="2"/>
+        <f>C23/H23</f>
         <v>2.9424983877037341</v>
       </c>
       <c r="F23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>6.2334236822732194</v>
       </c>
       <c r="G23">
@@ -2185,32 +2365,40 @@
         <v>5768</v>
       </c>
       <c r="I23">
+        <f t="shared" si="3"/>
+        <v>0.3093269918382448</v>
+      </c>
+      <c r="J23">
+        <f>H23/$H$48</f>
+        <v>0.47205172272690071</v>
+      </c>
+      <c r="K23">
         <v>51882</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <f t="shared" si="12"/>
         <v>13250</v>
       </c>
-      <c r="K23" s="2">
+      <c r="M23" s="2">
         <v>8395.8777711599105</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23" t="s">
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
         <v>21</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>33.299999999999997</v>
       </c>
-      <c r="O23" s="1">
+      <c r="Q23" s="1">
         <v>14358953</v>
       </c>
-      <c r="P23" s="1">
+      <c r="R23" s="1">
         <v>11309563</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1992</v>
       </c>
@@ -2218,20 +2406,20 @@
         <v>5250</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
-        <v>15944.842051347208</v>
+        <f t="shared" si="1"/>
+        <v>15944.842051347207</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
-        <v>32536.744326221033</v>
+        <f t="shared" si="2"/>
+        <v>32536.744326221029</v>
       </c>
       <c r="E24">
-        <f t="shared" si="2"/>
-        <v>2.6627992737720789</v>
+        <f>C24/H24</f>
+        <v>2.6627992737720785</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
-        <v>5.4336580371110612</v>
+        <f t="shared" si="0"/>
+        <v>5.4336580371110603</v>
       </c>
       <c r="G24">
         <v>4197.5666666666666</v>
@@ -2240,32 +2428,40 @@
         <v>5988</v>
       </c>
       <c r="I24">
+        <f t="shared" si="3"/>
+        <v>0.3292600819182413</v>
+      </c>
+      <c r="J24">
+        <f>H24/$H$48</f>
+        <v>0.49005646943285047</v>
+      </c>
+      <c r="K24">
         <v>44290</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <f t="shared" si="12"/>
         <v>13250</v>
       </c>
-      <c r="K24" s="2">
+      <c r="M24" s="2">
         <v>8734.8511773709688</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24" t="s">
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
         <v>21</v>
       </c>
-      <c r="N24">
+      <c r="P24">
         <v>34.4</v>
       </c>
-      <c r="O24" s="1">
+      <c r="Q24" s="1">
         <v>14487359</v>
       </c>
-      <c r="P24" s="1">
+      <c r="R24" s="1">
         <v>11384567</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1993</v>
       </c>
@@ -2273,19 +2469,19 @@
         <v>5250</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
-        <v>15033.645116970338</v>
+        <f t="shared" si="1"/>
+        <v>15033.645116970336</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28919.412733668221</v>
       </c>
       <c r="E25">
-        <f t="shared" si="2"/>
-        <v>2.3667577325205191</v>
+        <f>C25/H25</f>
+        <v>2.3667577325205187</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>4.5528042716732084</v>
       </c>
       <c r="G25">
@@ -2295,32 +2491,40 @@
         <v>6352</v>
       </c>
       <c r="I25">
+        <f t="shared" si="3"/>
+        <v>0.34921670420925893</v>
+      </c>
+      <c r="J25">
+        <f>H25/$H$48</f>
+        <v>0.51984614125542183</v>
+      </c>
+      <c r="K25">
         <v>35818</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <f>2625+3500+5500+5500</f>
         <v>17125</v>
       </c>
-      <c r="K25" s="2">
+      <c r="M25" s="2">
         <v>11776.43353729859</v>
       </c>
-      <c r="L25">
+      <c r="N25">
         <v>1</v>
       </c>
-      <c r="M25" t="s">
+      <c r="O25" t="s">
         <v>21</v>
       </c>
-      <c r="N25">
+      <c r="P25">
         <v>34</v>
       </c>
-      <c r="O25" s="1">
+      <c r="Q25" s="1">
         <v>14304803</v>
       </c>
-      <c r="P25" s="1">
+      <c r="R25" s="1">
         <v>11189088</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1994</v>
       </c>
@@ -2328,20 +2532,20 @@
         <v>5250</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>14177.108284864476</v>
+        <f t="shared" si="1"/>
+        <v>14177.108284864478</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
-        <v>26548.672204254257</v>
+        <f t="shared" si="2"/>
+        <v>26548.672204254261</v>
       </c>
       <c r="E26">
-        <f t="shared" si="2"/>
-        <v>2.1727369018949387</v>
+        <f>C26/H26</f>
+        <v>2.1727369018949392</v>
       </c>
       <c r="F26">
-        <f t="shared" si="3"/>
-        <v>4.0687620236404989</v>
+        <f t="shared" si="0"/>
+        <v>4.0687620236404998</v>
       </c>
       <c r="G26">
         <v>4720.958333333333</v>
@@ -2350,32 +2554,40 @@
         <v>6525</v>
       </c>
       <c r="I26">
+        <f t="shared" si="3"/>
+        <v>0.37031529240733213</v>
+      </c>
+      <c r="J26">
+        <f>H26/$H$48</f>
+        <v>0.53400441934691878</v>
+      </c>
+      <c r="K26">
         <v>42843</v>
       </c>
-      <c r="J26">
-        <f t="shared" ref="J26:J38" si="15">2625+3500+5500+5500</f>
+      <c r="L26">
+        <f t="shared" ref="L26:L38" si="15">2625+3500+5500+5500</f>
         <v>17125</v>
       </c>
-      <c r="K26" s="2">
+      <c r="M26" s="2">
         <v>15593.929353736819</v>
       </c>
-      <c r="L26">
+      <c r="N26">
         <v>1</v>
       </c>
-      <c r="M26" t="s">
+      <c r="O26" t="s">
         <v>21</v>
       </c>
-      <c r="N26">
+      <c r="P26">
         <v>34.6</v>
       </c>
-      <c r="O26" s="1">
+      <c r="Q26" s="1">
         <v>14278790</v>
       </c>
-      <c r="P26" s="1">
+      <c r="R26" s="1">
         <v>11133680</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1995</v>
       </c>
@@ -2383,20 +2595,20 @@
         <v>5250</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13486.788679321324</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
-        <v>24188.326856396194</v>
+        <f t="shared" si="2"/>
+        <v>24188.32685639619</v>
       </c>
       <c r="E27">
-        <f t="shared" si="2"/>
+        <f>C27/H27</f>
         <v>1.9795668104097055</v>
       </c>
       <c r="F27">
-        <f t="shared" si="3"/>
-        <v>3.5503195151029199</v>
+        <f t="shared" si="0"/>
+        <v>3.5503195151029194</v>
       </c>
       <c r="G27">
         <v>4962.5999999999995</v>
@@ -2405,40 +2617,48 @@
         <v>6813</v>
       </c>
       <c r="I27">
+        <f t="shared" si="3"/>
+        <v>0.38926983471236448</v>
+      </c>
+      <c r="J27">
+        <f>H27/$H$48</f>
+        <v>0.5575742695801621</v>
+      </c>
+      <c r="K27">
         <v>51832</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K27" s="2">
+      <c r="M27" s="2">
         <v>18104.599209</v>
       </c>
-      <c r="L27">
+      <c r="N27">
         <v>1</v>
       </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>21</v>
       </c>
-      <c r="N27">
+      <c r="P27">
         <v>34.299999999999997</v>
       </c>
-      <c r="O27" s="1">
+      <c r="Q27" s="1">
         <v>14261781</v>
       </c>
-      <c r="P27" s="1">
+      <c r="R27" s="1">
         <v>11092374</v>
       </c>
-      <c r="T27" s="1">
-        <f t="shared" ref="T27" si="16">AVERAGE(P27:P31)</f>
+      <c r="V27" s="1">
+        <f t="shared" ref="V27" si="16">AVERAGE(R27:R31)</f>
         <v>11184500</v>
       </c>
-      <c r="U27">
-        <f t="shared" ref="U27" si="17">T27-T22</f>
+      <c r="W27">
+        <f t="shared" ref="W27" si="17">V27-V22</f>
         <v>12177</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1996</v>
       </c>
@@ -2446,20 +2666,20 @@
         <v>5250</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12761.609560309651</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
-        <v>22372.181810247293</v>
+        <f t="shared" si="2"/>
+        <v>22372.18181024729</v>
       </c>
       <c r="E28">
-        <f t="shared" si="2"/>
+        <f>C28/H28</f>
         <v>1.8309339397861766</v>
       </c>
       <c r="F28">
-        <f t="shared" si="3"/>
-        <v>3.209782182244949</v>
+        <f t="shared" si="0"/>
+        <v>3.2097821822449482</v>
       </c>
       <c r="G28">
         <v>5244.5999999999995</v>
@@ -2468,32 +2688,40 @@
         <v>6970</v>
       </c>
       <c r="I28">
+        <f t="shared" si="3"/>
+        <v>0.41139011307227397</v>
+      </c>
+      <c r="J28">
+        <f>H28/$H$48</f>
+        <v>0.57042311154758985</v>
+      </c>
+      <c r="K28">
         <v>58327</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K28" s="2">
+      <c r="M28" s="2">
         <v>19946.724761000001</v>
       </c>
-      <c r="L28">
+      <c r="N28">
         <v>1</v>
       </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
         <v>21</v>
       </c>
-      <c r="N28">
+      <c r="P28">
         <v>35.5</v>
       </c>
-      <c r="O28" s="1">
+      <c r="Q28" s="1">
         <v>14367520</v>
       </c>
-      <c r="P28" s="1">
+      <c r="R28" s="1">
         <v>11120499</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1997</v>
       </c>
@@ -2501,19 +2729,19 @@
         <v>5250</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12088.162651599754</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20707.312412715182</v>
       </c>
       <c r="E29">
-        <f t="shared" si="2"/>
+        <f>C29/H29</f>
         <v>1.6946814315995731</v>
       </c>
       <c r="F29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>2.9030299190684401</v>
       </c>
       <c r="G29">
@@ -2523,32 +2751,40 @@
         <v>7133</v>
       </c>
       <c r="I29">
+        <f t="shared" si="3"/>
+        <v>0.43430917926184687</v>
+      </c>
+      <c r="J29">
+        <f>H29/$H$48</f>
+        <v>0.58376299206154347</v>
+      </c>
+      <c r="K29">
         <v>80547</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K29" s="2">
+      <c r="M29" s="2">
         <v>21085.003477999999</v>
       </c>
-      <c r="L29">
+      <c r="N29">
         <v>1</v>
       </c>
-      <c r="M29" t="s">
+      <c r="O29" t="s">
         <v>21</v>
       </c>
-      <c r="N29">
+      <c r="P29">
         <v>36.799999999999997</v>
       </c>
-      <c r="O29" s="1">
+      <c r="Q29" s="1">
         <v>14502334</v>
       </c>
-      <c r="P29" s="1">
+      <c r="R29" s="1">
         <v>11196119</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1998</v>
       </c>
@@ -2556,19 +2792,19 @@
         <v>5250</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11387.900378578415</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18821.690075185939</v>
       </c>
       <c r="E30">
-        <f t="shared" si="2"/>
+        <f>C30/H30</f>
         <v>1.5403625562800507</v>
       </c>
       <c r="F30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>2.5458798965488896</v>
       </c>
       <c r="G30">
@@ -2578,32 +2814,40 @@
         <v>7393</v>
       </c>
       <c r="I30">
+        <f t="shared" si="3"/>
+        <v>0.46101562408077307</v>
+      </c>
+      <c r="J30">
+        <f>H30/$H$48</f>
+        <v>0.60504132907766595</v>
+      </c>
+      <c r="K30">
         <v>91360</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K30" s="2">
+      <c r="M30" s="2">
         <v>21712.867800000004</v>
       </c>
-      <c r="L30">
+      <c r="N30">
         <v>1</v>
       </c>
-      <c r="M30" t="s">
+      <c r="O30" t="s">
         <v>21</v>
       </c>
-      <c r="N30">
+      <c r="P30">
         <v>36.5</v>
       </c>
-      <c r="O30" s="1">
+      <c r="Q30" s="1">
         <v>14506967</v>
       </c>
-      <c r="P30" s="1">
+      <c r="R30" s="1">
         <v>11137769</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1999</v>
       </c>
@@ -2611,19 +2855,19 @@
         <v>5250</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10659.12553583989</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17400.648620230812</v>
       </c>
       <c r="E31">
-        <f t="shared" si="2"/>
+        <f>C31/H31</f>
         <v>1.4240648678476808</v>
       </c>
       <c r="F31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>2.3247359546066551</v>
       </c>
       <c r="G31">
@@ -2633,32 +2877,40 @@
         <v>7485</v>
       </c>
       <c r="I31">
+        <f t="shared" si="3"/>
+        <v>0.49253571339858732</v>
+      </c>
+      <c r="J31">
+        <f>H31/$H$48</f>
+        <v>0.61257058679106313</v>
+      </c>
+      <c r="K31">
         <v>116513</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K31" s="2">
+      <c r="M31" s="2">
         <v>22583.737441000001</v>
       </c>
-      <c r="L31">
+      <c r="N31">
         <v>1</v>
       </c>
-      <c r="M31" t="s">
+      <c r="O31" t="s">
         <v>21</v>
       </c>
-      <c r="N31">
+      <c r="P31">
         <v>35.6</v>
       </c>
-      <c r="O31" s="1">
+      <c r="Q31" s="1">
         <v>14849691</v>
       </c>
-      <c r="P31" s="1">
+      <c r="R31" s="1">
         <v>11375739</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -2666,19 +2918,19 @@
         <v>5250</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9897.6712288251529</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16229.152542272483</v>
       </c>
       <c r="E32">
-        <f t="shared" si="2"/>
+        <f>C32/H32</f>
         <v>1.3281899126174386</v>
       </c>
       <c r="F32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>2.1778250861879336</v>
       </c>
       <c r="G32">
@@ -2688,40 +2940,48 @@
         <v>7452</v>
       </c>
       <c r="I32">
+        <f t="shared" si="3"/>
+        <v>0.53042780252291444</v>
+      </c>
+      <c r="J32">
+        <f>H32/$H$48</f>
+        <v>0.60986987478517063</v>
+      </c>
+      <c r="K32">
         <v>133290</v>
       </c>
-      <c r="J32">
+      <c r="L32">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K32" s="2">
+      <c r="M32" s="2">
         <v>23694.724191000001</v>
       </c>
-      <c r="L32">
+      <c r="N32">
         <v>1</v>
       </c>
-      <c r="M32" t="s">
+      <c r="O32" t="s">
         <v>21</v>
       </c>
-      <c r="N32">
+      <c r="P32">
         <v>35.5</v>
       </c>
-      <c r="O32" s="1">
+      <c r="Q32" s="1">
         <v>15312289</v>
       </c>
-      <c r="P32" s="1">
+      <c r="R32" s="1">
         <v>11752786</v>
       </c>
-      <c r="T32" s="1">
-        <f t="shared" ref="T32" si="18">AVERAGE(P32:P36)</f>
+      <c r="V32" s="1">
+        <f t="shared" ref="V32" si="18">AVERAGE(R32:R36)</f>
         <v>12515349</v>
       </c>
-      <c r="U32">
-        <f t="shared" ref="U32" si="19">T32-T27</f>
+      <c r="W32">
+        <f t="shared" ref="W32" si="19">V32-V27</f>
         <v>1330849</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -2729,19 +2989,19 @@
         <v>5250</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9472.546103439654</v>
       </c>
       <c r="D33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15053.328240074019</v>
       </c>
       <c r="E33">
-        <f t="shared" si="2"/>
+        <f>C33/H33</f>
         <v>1.2319607365638774</v>
       </c>
       <c r="F33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1.9577745142507503</v>
       </c>
       <c r="G33">
@@ -2751,32 +3011,40 @@
         <v>7689</v>
       </c>
       <c r="I33">
+        <f t="shared" si="3"/>
+        <v>0.5542332486609518</v>
+      </c>
+      <c r="J33">
+        <f>H33/$H$48</f>
+        <v>0.62926589737294381</v>
+      </c>
+      <c r="K33">
         <v>161643</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K33" s="2">
+      <c r="M33" s="2">
         <v>25858.497605</v>
       </c>
-      <c r="L33">
+      <c r="N33">
         <v>1</v>
       </c>
-      <c r="M33" t="s">
+      <c r="O33" t="s">
         <v>21</v>
       </c>
-      <c r="N33">
+      <c r="P33">
         <v>36.299999999999997</v>
       </c>
-      <c r="O33" s="1">
+      <c r="Q33" s="1">
         <v>15927987</v>
       </c>
-      <c r="P33" s="1">
+      <c r="R33" s="1">
         <v>12233156</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2002</v>
       </c>
@@ -2784,20 +3052,20 @@
         <v>5250</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
-        <v>9115.1333186550783</v>
+        <f t="shared" si="1"/>
+        <v>9115.1333186550764</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
-        <v>13925.708179625706</v>
+        <f t="shared" si="2"/>
+        <v>13925.708179625704</v>
       </c>
       <c r="E34">
-        <f t="shared" si="2"/>
-        <v>1.1396765839778793</v>
+        <f>C34/H34</f>
+        <v>1.1396765839778791</v>
       </c>
       <c r="F34">
-        <f t="shared" si="3"/>
-        <v>1.7411488096556271</v>
+        <f t="shared" si="0"/>
+        <v>1.7411488096556269</v>
       </c>
       <c r="G34">
         <v>7342.6833333333334</v>
@@ -2806,32 +3074,40 @@
         <v>7998</v>
       </c>
       <c r="I34">
+        <f t="shared" si="3"/>
+        <v>0.57596524553901196</v>
+      </c>
+      <c r="J34">
+        <f>H34/$H$48</f>
+        <v>0.65455438251902776</v>
+      </c>
+      <c r="K34">
         <v>118352</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K34" s="2">
+      <c r="M34" s="2">
         <v>29237.889558000003</v>
       </c>
-      <c r="L34">
+      <c r="N34">
         <v>1</v>
       </c>
-      <c r="M34" t="s">
+      <c r="O34" t="s">
         <v>21</v>
       </c>
-      <c r="N34">
+      <c r="P34">
         <v>36.700000000000003</v>
       </c>
-      <c r="O34" s="1">
+      <c r="Q34" s="1">
         <v>16611711</v>
       </c>
-      <c r="P34" s="1">
+      <c r="R34" s="1">
         <v>12751993</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2003</v>
       </c>
@@ -2839,20 +3115,20 @@
         <v>5250</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
-        <v>8666.1399285477673</v>
+        <f t="shared" si="1"/>
+        <v>8666.1399285477655</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
-        <v>12288.680954731944</v>
+        <f t="shared" si="2"/>
+        <v>12288.680954731943</v>
       </c>
       <c r="E35">
-        <f t="shared" si="2"/>
-        <v>1.0057026724553519</v>
+        <f>C35/H35</f>
+        <v>1.0057026724553517</v>
       </c>
       <c r="F35">
-        <f t="shared" si="3"/>
-        <v>1.4260973604191649</v>
+        <f t="shared" si="0"/>
+        <v>1.4260973604191647</v>
       </c>
       <c r="G35">
         <v>7723.1083333333327</v>
@@ -2861,32 +3137,40 @@
         <v>8617</v>
       </c>
       <c r="I35">
+        <f t="shared" si="3"/>
+        <v>0.60580605013145361</v>
+      </c>
+      <c r="J35">
+        <f>H35/$H$48</f>
+        <v>0.70521319256894999</v>
+      </c>
+      <c r="K35">
         <v>107196</v>
       </c>
-      <c r="J35">
+      <c r="L35">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K35" s="2">
+      <c r="M35" s="2">
         <v>33729.110334000005</v>
       </c>
-      <c r="L35">
+      <c r="N35">
         <v>1</v>
       </c>
-      <c r="M35" t="s">
+      <c r="O35" t="s">
         <v>21</v>
       </c>
-      <c r="N35">
+      <c r="P35">
         <v>37.799999999999997</v>
       </c>
-      <c r="O35" s="1">
+      <c r="Q35" s="1">
         <v>16911481</v>
       </c>
-      <c r="P35" s="1">
+      <c r="R35" s="1">
         <v>12858698</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2004</v>
       </c>
@@ -2894,20 +3178,20 @@
         <v>5250</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8149.549983764914</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
-        <v>11044.737272806507</v>
+        <f t="shared" si="2"/>
+        <v>11044.737272806509</v>
       </c>
       <c r="E36">
-        <f t="shared" si="2"/>
+        <f>C36/H36</f>
         <v>0.90389862286656097</v>
       </c>
       <c r="F36">
-        <f t="shared" si="3"/>
-        <v>1.2250152254665603</v>
+        <f t="shared" si="0"/>
+        <v>1.2250152254665605</v>
       </c>
       <c r="G36">
         <v>8212.6666666666679</v>
@@ -2916,32 +3200,40 @@
         <v>9016</v>
       </c>
       <c r="I36">
+        <f t="shared" si="3"/>
+        <v>0.64420735015537811</v>
+      </c>
+      <c r="J36">
+        <f>H36/$H$48</f>
+        <v>0.73786725591292246</v>
+      </c>
+      <c r="K36">
         <v>139037</v>
       </c>
-      <c r="J36">
+      <c r="L36">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K36" s="2">
+      <c r="M36" s="2">
         <v>37174.845230999999</v>
       </c>
-      <c r="L36">
+      <c r="N36">
         <v>1</v>
       </c>
-      <c r="M36" t="s">
+      <c r="O36" t="s">
         <v>21</v>
       </c>
-      <c r="N36">
+      <c r="P36">
         <v>38</v>
       </c>
-      <c r="O36" s="1">
+      <c r="Q36" s="1">
         <v>17272044</v>
       </c>
-      <c r="P36" s="1">
+      <c r="R36" s="1">
         <v>12980112</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2005</v>
       </c>
@@ -2949,20 +3241,20 @@
         <v>5250</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
-        <v>7651.5968088592817</v>
+        <f t="shared" si="1"/>
+        <v>7651.5968088592826</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
-        <v>10086.833682970284</v>
+        <f t="shared" si="2"/>
+        <v>10086.833682970286</v>
       </c>
       <c r="E37">
-        <f t="shared" si="2"/>
-        <v>0.82550402512237364</v>
+        <f>C37/H37</f>
+        <v>0.82550402512237375</v>
       </c>
       <c r="F37">
-        <f t="shared" si="3"/>
-        <v>1.0882332164171198</v>
+        <f t="shared" si="0"/>
+        <v>1.08823321641712</v>
       </c>
       <c r="G37">
         <v>8747.1333333333332</v>
@@ -2971,40 +3263,48 @@
         <v>9269</v>
       </c>
       <c r="I37">
+        <f t="shared" si="3"/>
+        <v>0.68613129143466745</v>
+      </c>
+      <c r="J37">
+        <f>H37/$H$48</f>
+        <v>0.75857271462476472</v>
+      </c>
+      <c r="K37">
         <v>124374</v>
       </c>
-      <c r="J37">
+      <c r="L37">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K37" s="2">
+      <c r="M37" s="2">
         <v>39261.861787000002</v>
       </c>
-      <c r="L37">
+      <c r="N37">
         <v>1</v>
       </c>
-      <c r="M37" t="s">
+      <c r="O37" t="s">
         <v>21</v>
       </c>
-      <c r="N37">
+      <c r="P37">
         <v>38.9</v>
       </c>
-      <c r="O37" s="1">
+      <c r="Q37" s="1">
         <v>17487475</v>
       </c>
-      <c r="P37" s="1">
+      <c r="R37" s="1">
         <v>13021834</v>
       </c>
-      <c r="T37" s="1">
-        <f t="shared" ref="T37" si="20">AVERAGE(P37:P41)</f>
+      <c r="V37" s="1">
+        <f t="shared" ref="V37" si="20">AVERAGE(R37:R41)</f>
         <v>13695941.6</v>
       </c>
-      <c r="U37">
-        <f t="shared" ref="U37" si="21">T37-T32</f>
+      <c r="W37">
+        <f t="shared" ref="W37" si="21">V37-V32</f>
         <v>1180592.5999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2006</v>
       </c>
@@ -3012,19 +3312,19 @@
         <v>5250</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7227.5386459475076</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9181.1305452575725</v>
       </c>
       <c r="E38">
-        <f t="shared" si="2"/>
+        <f>C38/H38</f>
         <v>0.75138149973464052</v>
       </c>
       <c r="F38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.95447869271832542</v>
       </c>
       <c r="G38">
@@ -3034,32 +3334,40 @@
         <v>9619</v>
       </c>
       <c r="I38">
+        <f t="shared" si="3"/>
+        <v>0.72638836776662319</v>
+      </c>
+      <c r="J38">
+        <f>H38/$H$48</f>
+        <v>0.78721662983877572</v>
+      </c>
+      <c r="K38">
         <v>135861</v>
       </c>
-      <c r="J38">
+      <c r="L38">
         <f t="shared" si="15"/>
         <v>17125</v>
       </c>
-      <c r="K38" s="2">
+      <c r="M38" s="2">
         <v>39865.693807000003</v>
       </c>
-      <c r="L38">
+      <c r="N38">
         <v>1</v>
       </c>
-      <c r="M38" t="s">
+      <c r="O38" t="s">
         <v>21</v>
       </c>
-      <c r="N38">
+      <c r="P38">
         <v>37.299999999999997</v>
       </c>
-      <c r="O38" s="1">
+      <c r="Q38" s="1">
         <v>17754230</v>
       </c>
-      <c r="P38" s="1">
+      <c r="R38" s="1">
         <v>13175350</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2007</v>
       </c>
@@ -3067,19 +3375,19 @@
         <v>5250</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6895.3850155953396</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8664.614305384559</v>
       </c>
       <c r="E39">
-        <f t="shared" si="2"/>
+        <f>C39/H39</f>
         <v>0.70910993578726245</v>
       </c>
       <c r="F39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.8910545357244507</v>
       </c>
       <c r="G39">
@@ -3089,32 +3397,40 @@
         <v>9724</v>
       </c>
       <c r="I39">
+        <f t="shared" si="3"/>
+        <v>0.76137880453753326</v>
+      </c>
+      <c r="J39">
+        <f>H39/$H$48</f>
+        <v>0.79580980440297899</v>
+      </c>
+      <c r="K39">
         <v>154692</v>
       </c>
-      <c r="J39">
+      <c r="L39">
         <f>3500+4500+5500+5500</f>
         <v>19000</v>
       </c>
-      <c r="K39" s="2">
+      <c r="M39" s="2">
         <v>43820.560598000004</v>
       </c>
-      <c r="L39">
+      <c r="N39">
         <v>1</v>
       </c>
-      <c r="M39" t="s">
+      <c r="O39" t="s">
         <v>21</v>
       </c>
-      <c r="N39">
+      <c r="P39">
         <v>38.799999999999997</v>
       </c>
-      <c r="O39" s="1">
+      <c r="Q39" s="1">
         <v>18258138</v>
       </c>
-      <c r="P39" s="1">
+      <c r="R39" s="1">
         <v>13500894</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2008</v>
       </c>
@@ -3122,20 +3438,20 @@
         <v>5250</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
-        <v>6708.8313174513005</v>
+        <f t="shared" si="1"/>
+        <v>6708.8313174512996</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
-        <v>8155.1143919555752</v>
+        <f t="shared" si="2"/>
+        <v>8155.1143919555743</v>
       </c>
       <c r="E40">
-        <f t="shared" si="2"/>
+        <f>C40/H40</f>
         <v>0.66741258629638878</v>
       </c>
       <c r="F40">
-        <f t="shared" si="3"/>
-        <v>0.81129271706681017</v>
+        <f t="shared" si="0"/>
+        <v>0.81129271706681005</v>
       </c>
       <c r="G40">
         <v>9976.3333333333339</v>
@@ -3144,32 +3460,40 @@
         <v>10052</v>
       </c>
       <c r="I40">
+        <f t="shared" si="3"/>
+        <v>0.78255060405878363</v>
+      </c>
+      <c r="J40">
+        <f>H40/$H$48</f>
+        <v>0.82265324494639491</v>
+      </c>
+      <c r="K40">
         <v>130183</v>
       </c>
-      <c r="J40">
-        <f t="shared" ref="J40:J49" si="22">3500+4500+5500+5500</f>
+      <c r="L40">
+        <f t="shared" ref="L40:L49" si="22">3500+4500+5500+5500</f>
         <v>19000</v>
       </c>
-      <c r="K40" s="2">
+      <c r="M40" s="2">
         <v>57913.02765051715</v>
       </c>
-      <c r="L40">
+      <c r="N40">
         <v>1</v>
       </c>
-      <c r="M40" t="s">
+      <c r="O40" t="s">
         <v>21</v>
       </c>
-      <c r="N40">
+      <c r="P40">
         <v>39.6</v>
       </c>
-      <c r="O40" s="1">
+      <c r="Q40" s="1">
         <v>19081686</v>
       </c>
-      <c r="P40" s="1">
+      <c r="R40" s="1">
         <v>13970862</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2009</v>
       </c>
@@ -3177,19 +3501,19 @@
         <v>5250</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6800.2676402528905</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8124.8137573335362</v>
       </c>
       <c r="E41">
-        <f t="shared" si="2"/>
+        <f>C41/H41</f>
         <v>0.66493278969911906</v>
       </c>
       <c r="F41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.79444741931490526</v>
       </c>
       <c r="G41">
@@ -3199,32 +3523,40 @@
         <v>10227</v>
       </c>
       <c r="I41">
+        <f t="shared" si="3"/>
+        <v>0.77202843736967408</v>
+      </c>
+      <c r="J41">
+        <f>H41/$H$48</f>
+        <v>0.83697520255340041</v>
+      </c>
+      <c r="K41">
         <v>110988</v>
       </c>
-      <c r="J41">
+      <c r="L41">
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K41" s="2">
+      <c r="M41" s="2">
         <v>67681.483983686572</v>
       </c>
-      <c r="L41">
+      <c r="N41">
         <v>1</v>
       </c>
-      <c r="M41" t="s">
+      <c r="O41" t="s">
         <v>22</v>
       </c>
-      <c r="N41">
+      <c r="P41">
         <v>41.3</v>
       </c>
-      <c r="O41" s="1">
+      <c r="Q41" s="1">
         <v>20313594</v>
       </c>
-      <c r="P41" s="1">
+      <c r="R41" s="1">
         <v>14810768</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2010</v>
       </c>
@@ -3232,19 +3564,19 @@
         <v>5250</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6570.8347855112715</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
-        <v>7640.0257154974042</v>
+        <f t="shared" si="2"/>
+        <v>7640.0257154974051</v>
       </c>
       <c r="E42">
-        <f t="shared" si="2"/>
+        <f>C42/H42</f>
         <v>0.62525785379306043</v>
       </c>
       <c r="F42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.72699835526666712</v>
       </c>
       <c r="G42">
@@ -3254,40 +3586,48 @@
         <v>10509</v>
       </c>
       <c r="I42">
+        <f t="shared" si="3"/>
+        <v>0.79898523876696459</v>
+      </c>
+      <c r="J42">
+        <f>H42/$H$48</f>
+        <v>0.86005401424011785</v>
+      </c>
+      <c r="K42">
         <v>117828</v>
       </c>
-      <c r="J42">
+      <c r="L42">
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K42" s="2">
+      <c r="M42" s="2">
         <v>70899.286510563674</v>
       </c>
-      <c r="L42">
+      <c r="N42">
         <v>1</v>
       </c>
-      <c r="M42" t="s">
+      <c r="O42" t="s">
         <v>22</v>
       </c>
-      <c r="N42">
+      <c r="P42">
         <v>41.2</v>
       </c>
-      <c r="O42" s="1">
+      <c r="Q42" s="1">
         <v>21019438</v>
       </c>
-      <c r="P42" s="1">
+      <c r="R42" s="1">
         <v>15142171</v>
       </c>
-      <c r="T42" s="1">
-        <f t="shared" ref="T42" si="23">AVERAGE(P42:P46)</f>
+      <c r="V42" s="1">
+        <f t="shared" ref="V42" si="23">AVERAGE(R42:R46)</f>
         <v>14908929.800000001</v>
       </c>
-      <c r="U42">
-        <f t="shared" ref="U42" si="24">T42-T37</f>
+      <c r="W42">
+        <f t="shared" ref="W42" si="24">V42-V37</f>
         <v>1212988.2000000011</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -3295,19 +3635,19 @@
         <v>5250</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6289.7050358867109</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7080.6988975031991</v>
       </c>
       <c r="E43">
-        <f t="shared" si="2"/>
+        <f>C43/H43</f>
         <v>0.57948268250292156</v>
       </c>
       <c r="F43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.65235847590779428</v>
       </c>
       <c r="G43">
@@ -3317,32 +3657,40 @@
         <v>10854</v>
       </c>
       <c r="I43">
+        <f t="shared" si="3"/>
+        <v>0.83469733000919089</v>
+      </c>
+      <c r="J43">
+        <f>H43/$H$48</f>
+        <v>0.88828873066535718</v>
+      </c>
+      <c r="K43">
         <v>129552</v>
       </c>
-      <c r="J43">
+      <c r="L43">
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K43" s="2">
+      <c r="M43" s="2">
         <v>71294.597505559141</v>
       </c>
-      <c r="L43">
+      <c r="N43">
         <v>1</v>
       </c>
-      <c r="M43" t="s">
+      <c r="O43" t="s">
         <v>22</v>
       </c>
-      <c r="N43">
+      <c r="P43">
         <v>42</v>
       </c>
-      <c r="O43" s="1">
+      <c r="Q43" s="1">
         <v>21010590</v>
       </c>
-      <c r="P43" s="1">
+      <c r="R43" s="1">
         <v>15116303</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2012</v>
       </c>
@@ -3350,19 +3698,19 @@
         <v>5250</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6080.7305921553198</v>
       </c>
       <c r="D44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6632.1920115634966</v>
       </c>
       <c r="E44">
-        <f t="shared" si="2"/>
+        <f>C44/H44</f>
         <v>0.54277698760647319</v>
       </c>
       <c r="F44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.59200142922105659</v>
       </c>
       <c r="G44">
@@ -3372,32 +3720,40 @@
         <v>11203</v>
       </c>
       <c r="I44">
+        <f t="shared" si="3"/>
+        <v>0.86338309524400969</v>
+      </c>
+      <c r="J44">
+        <f>H44/$H$48</f>
+        <v>0.91685080612161385</v>
+      </c>
+      <c r="K44">
         <v>135991</v>
       </c>
-      <c r="J44">
+      <c r="L44">
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K44" s="2">
+      <c r="M44" s="2">
         <v>67937.063653967853</v>
       </c>
-      <c r="L44">
+      <c r="N44">
         <v>1</v>
       </c>
-      <c r="M44" t="s">
+      <c r="O44" t="s">
         <v>22</v>
       </c>
-      <c r="N44">
+      <c r="P44">
         <v>41</v>
       </c>
-      <c r="O44" s="1">
+      <c r="Q44" s="1">
         <v>20644478</v>
       </c>
-      <c r="P44" s="1">
+      <c r="R44" s="1">
         <v>14884667</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2013</v>
       </c>
@@ -3405,20 +3761,20 @@
         <v>5250</v>
       </c>
       <c r="C45">
-        <f t="shared" si="0"/>
-        <v>5913.9661311985301</v>
+        <f t="shared" si="1"/>
+        <v>5913.9661311985292</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
-        <v>6319.4361309239039</v>
+        <f t="shared" si="2"/>
+        <v>6319.4361309239021</v>
       </c>
       <c r="E45">
-        <f t="shared" si="2"/>
+        <f>C45/H45</f>
         <v>0.51718112209869083</v>
       </c>
       <c r="F45">
-        <f t="shared" si="3"/>
-        <v>0.55263980156745984</v>
+        <f t="shared" si="0"/>
+        <v>0.55263980156745973</v>
       </c>
       <c r="G45">
         <v>11317.199999999999</v>
@@ -3427,32 +3783,40 @@
         <v>11435</v>
       </c>
       <c r="I45">
+        <f t="shared" si="3"/>
+        <v>0.88772912856300557</v>
+      </c>
+      <c r="J45">
+        <f>H45/$H$48</f>
+        <v>0.93583762992061548</v>
+      </c>
+      <c r="K45">
         <v>153794</v>
       </c>
-      <c r="J45">
+      <c r="L45">
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K45" s="2">
+      <c r="M45" s="2">
         <v>65652.303782821924</v>
       </c>
-      <c r="L45">
+      <c r="N45">
         <v>1</v>
       </c>
-      <c r="M45" t="s">
+      <c r="O45" t="s">
         <v>22</v>
       </c>
-      <c r="N45">
+      <c r="P45">
         <v>39.9</v>
       </c>
-      <c r="O45" s="1">
+      <c r="Q45" s="1">
         <v>20376677</v>
       </c>
-      <c r="P45" s="1">
+      <c r="R45" s="1">
         <v>14746848</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2014</v>
       </c>
@@ -3460,20 +3824,20 @@
         <v>5250</v>
       </c>
       <c r="C46">
-        <f t="shared" si="0"/>
-        <v>5661.0803324099725</v>
+        <f t="shared" si="1"/>
+        <v>5661.0803324099716</v>
       </c>
       <c r="D46">
-        <f t="shared" si="1"/>
-        <v>5873.0464070060671</v>
+        <f t="shared" si="2"/>
+        <v>5873.0464070060661</v>
       </c>
       <c r="E46">
-        <f t="shared" si="2"/>
-        <v>0.48064869522923864</v>
+        <f>C46/H46</f>
+        <v>0.48064869522923853</v>
       </c>
       <c r="F46">
-        <f t="shared" si="3"/>
-        <v>0.49864547520853009</v>
+        <f t="shared" si="0"/>
+        <v>0.49864547520852998</v>
       </c>
       <c r="G46">
         <v>11822.75</v>
@@ -3482,32 +3846,40 @@
         <v>11778</v>
       </c>
       <c r="I46">
+        <f t="shared" si="3"/>
+        <v>0.92738482616886464</v>
+      </c>
+      <c r="J46">
+        <f>H46/$H$48</f>
+        <v>0.96390866683034615</v>
+      </c>
+      <c r="K46">
         <v>162239</v>
       </c>
-      <c r="J46">
+      <c r="L46">
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K46" s="2">
+      <c r="M46" s="2">
         <v>62423.127847651929</v>
       </c>
-      <c r="L46">
+      <c r="N46">
         <v>1</v>
       </c>
-      <c r="M46" t="s">
+      <c r="O46" t="s">
         <v>22</v>
       </c>
-      <c r="N46">
+      <c r="P46">
         <v>40</v>
       </c>
-      <c r="O46" s="1">
+      <c r="Q46" s="1">
         <v>20209092</v>
       </c>
-      <c r="P46" s="1">
+      <c r="R46" s="1">
         <v>14654660</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2015</v>
       </c>
@@ -3515,19 +3887,19 @@
         <v>5250</v>
       </c>
       <c r="C47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5448.3913377061317</v>
       </c>
       <c r="D47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5511.0839201515919</v>
       </c>
       <c r="E47">
-        <f t="shared" si="2"/>
+        <f>C47/H47</f>
         <v>0.45102577298891816</v>
       </c>
       <c r="F47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.45621555630393973</v>
       </c>
       <c r="G47">
@@ -3537,40 +3909,48 @@
         <v>12080</v>
       </c>
       <c r="I47">
+        <f t="shared" si="3"/>
+        <v>0.96358717180736542</v>
+      </c>
+      <c r="J47">
+        <f>H47/$H$48</f>
+        <v>0.98862427367214989</v>
+      </c>
+      <c r="K47">
         <v>173799</v>
       </c>
-      <c r="J47">
+      <c r="L47">
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K47" s="2">
+      <c r="M47" s="2">
         <v>59815.726707200003</v>
       </c>
-      <c r="L47">
+      <c r="N47">
         <v>1</v>
       </c>
-      <c r="M47" t="s">
+      <c r="O47" t="s">
         <v>22</v>
       </c>
-      <c r="N47">
+      <c r="P47">
         <v>40.5</v>
       </c>
-      <c r="O47" s="1">
+      <c r="Q47" s="1">
         <v>19988204</v>
       </c>
-      <c r="P47" s="1">
+      <c r="R47" s="1">
         <v>14572843</v>
       </c>
-      <c r="T47" s="1">
-        <f t="shared" ref="T47" si="25">AVERAGE(P47:P51)</f>
+      <c r="V47" s="1">
+        <f t="shared" ref="V47" si="25">AVERAGE(R47:R51)</f>
         <v>14572946</v>
       </c>
-      <c r="U47">
-        <f t="shared" ref="U47" si="26">T47-T42</f>
+      <c r="W47">
+        <f t="shared" ref="W47" si="26">V47-V42</f>
         <v>-335983.80000000075</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2016</v>
       </c>
@@ -3578,11 +3958,11 @@
         <v>5250</v>
       </c>
       <c r="C48">
-        <f>B48*($G$48/G48)</f>
+        <f t="shared" si="1"/>
         <v>5250</v>
       </c>
       <c r="D48">
-        <f>C48*($H$48/H48)</f>
+        <f t="shared" si="2"/>
         <v>5250</v>
       </c>
       <c r="E48">
@@ -3600,32 +3980,40 @@
         <v>12219</v>
       </c>
       <c r="I48">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <f>H48/$H$48</f>
+        <v>1</v>
+      </c>
+      <c r="K48">
         <v>181351</v>
       </c>
-      <c r="J48">
+      <c r="L48">
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K48" s="2">
+      <c r="M48" s="2">
         <v>57805.074495200002</v>
       </c>
-      <c r="L48">
+      <c r="N48">
         <v>1</v>
       </c>
-      <c r="M48" t="s">
+      <c r="O48" t="s">
         <v>22</v>
       </c>
-      <c r="N48">
+      <c r="P48">
         <v>41.2</v>
       </c>
-      <c r="O48" s="1">
+      <c r="Q48" s="1">
         <v>19846904</v>
       </c>
-      <c r="P48" s="1">
+      <c r="R48" s="1">
         <v>14585840</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2017</v>
       </c>
@@ -3633,74 +4021,106 @@
         <v>5250</v>
       </c>
       <c r="C49">
-        <f>B49*($G$48/G49)</f>
-        <v>4781.1422887206982</v>
+        <f t="shared" si="1"/>
+        <v>4781.1422887206973</v>
       </c>
       <c r="G49">
         <v>13998.65</v>
       </c>
       <c r="I49">
+        <f t="shared" si="3"/>
+        <v>1.0980639527054854</v>
+      </c>
+      <c r="J49">
+        <f>H49/$H$48</f>
+        <v>0</v>
+      </c>
+      <c r="K49">
         <v>180440</v>
       </c>
-      <c r="J49">
+      <c r="L49">
         <f t="shared" si="22"/>
         <v>19000</v>
       </c>
-      <c r="K49" s="2">
+      <c r="M49" s="2">
         <v>55808.355549400003</v>
       </c>
-      <c r="L49">
+      <c r="N49">
         <v>1</v>
       </c>
-      <c r="M49" t="s">
+      <c r="O49" t="s">
         <v>22</v>
       </c>
-      <c r="O49" s="1">
+      <c r="Q49" s="1">
         <v>19765598</v>
       </c>
-      <c r="P49">
+      <c r="R49">
         <v>14560155</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2018</v>
       </c>
       <c r="B50">
         <v>5250</v>
       </c>
-      <c r="L50">
+      <c r="I50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <f>H50/$H$48</f>
+        <v>0</v>
+      </c>
+      <c r="N50">
         <v>1</v>
       </c>
-      <c r="M50" t="s">
+      <c r="O50" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2019</v>
       </c>
       <c r="B51">
         <v>5250</v>
       </c>
-      <c r="L51">
+      <c r="I51">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <f>H51/$H$48</f>
+        <v>0</v>
+      </c>
+      <c r="N51">
         <v>1</v>
       </c>
-      <c r="M51" t="s">
+      <c r="O51" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2020</v>
       </c>
       <c r="B52">
         <v>5250</v>
       </c>
-      <c r="L52">
+      <c r="I52">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <f>H52/$H$48</f>
+        <v>0</v>
+      </c>
+      <c r="N52">
         <v>1</v>
       </c>
-      <c r="M52" t="s">
+      <c r="O52" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cpe to cpi typo fix
</commit_message>
<xml_diff>
--- a/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
+++ b/papers/section-127-effects/data/section-127-effects-with-formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\research-dissertation-case-for-alt-ed\papers\section-127-effects\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E1B70D-751A-4FEE-A0CA-E5C31DF4942E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86B86FC-9C4D-4C62-8397-C7CE5BBDB355}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>2016-Based Education-Specific Deflator</t>
   </si>
   <si>
-    <t>CPE-Adjusted Average Tuition and Fees - All Institutions</t>
-  </si>
-  <si>
     <t>Nominal Adjusted Average Tuition and Fees - All Institutions</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Is H1 Edge Case</t>
+  </si>
+  <si>
+    <t>CPI-Adjusted Average Tuition and Fees - All Institutions</t>
   </si>
 </sst>
 </file>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,10 +1027,10 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
         <v>28</v>
@@ -1039,19 +1039,19 @@
         <v>29</v>
       </c>
       <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
         <v>35</v>
-      </c>
-      <c r="O1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" t="s">
-        <v>36</v>
       </c>
       <c r="Q1" t="s">
         <v>14</v>
@@ -1162,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C49" si="3">B3/J3</f>
+        <f t="shared" ref="C3:C48" si="3">B3/J3</f>
         <v>0</v>
       </c>
       <c r="D3">
@@ -1187,7 +1187,7 @@
         <v>4268</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J52" si="5">G3/$G$48</f>
+        <f t="shared" ref="J3:J48" si="5">G3/$G$48</f>
         <v>5.4902609329998728E-2</v>
       </c>
       <c r="K3">
@@ -2582,7 +2582,7 @@
         <v>5368437</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24:M52" si="17">N24+O24</f>
+        <f t="shared" ref="M24:M51" si="17">N24+O24</f>
         <v>51667</v>
       </c>
       <c r="N24">
@@ -3381,7 +3381,7 @@
         <v>0.57596524553901196</v>
       </c>
       <c r="K34">
-        <f t="shared" ref="K34:K52" si="23">I34/$I$48</f>
+        <f t="shared" ref="K34:K48" si="23">I34/$I$48</f>
         <v>0.65455438251902776</v>
       </c>
       <c r="L34">
@@ -3954,7 +3954,7 @@
         <v>5804182</v>
       </c>
       <c r="M41">
-        <f>N41+O41</f>
+        <f t="shared" ref="M41:M46" si="27">N41+O41</f>
         <v>111116</v>
       </c>
       <c r="N41">
@@ -4034,7 +4034,7 @@
         <v>6422751</v>
       </c>
       <c r="M42">
-        <f>N42+O42</f>
+        <f t="shared" si="27"/>
         <v>117914</v>
       </c>
       <c r="N42">
@@ -4070,11 +4070,11 @@
         <v>15142171</v>
       </c>
       <c r="AA42" s="1">
-        <f t="shared" ref="AA42" si="27">AVERAGE(W42:W46)</f>
+        <f t="shared" ref="AA42" si="28">AVERAGE(W42:W46)</f>
         <v>14908929.800000001</v>
       </c>
       <c r="AB42">
-        <f t="shared" ref="AB42" si="28">AA42-AA37</f>
+        <f t="shared" ref="AB42" si="29">AA42-AA37</f>
         <v>1212988.2000000011</v>
       </c>
     </row>
@@ -4122,7 +4122,7 @@
         <v>7507939</v>
       </c>
       <c r="M43">
-        <f>N43+O43</f>
+        <f t="shared" si="27"/>
         <v>129559</v>
       </c>
       <c r="N43">
@@ -4202,7 +4202,7 @@
         <v>8927090</v>
       </c>
       <c r="M44">
-        <f>N44+O44</f>
+        <f t="shared" si="27"/>
         <v>135994</v>
       </c>
       <c r="N44">
@@ -4282,7 +4282,7 @@
         <v>9164349</v>
       </c>
       <c r="M45">
-        <f>N45+O45</f>
+        <f t="shared" si="27"/>
         <v>153794</v>
       </c>
       <c r="N45">
@@ -4362,7 +4362,7 @@
         <v>9932480</v>
       </c>
       <c r="M46">
-        <f>N46+O46</f>
+        <f t="shared" si="27"/>
         <v>162239</v>
       </c>
       <c r="N46">
@@ -4478,11 +4478,11 @@
         <v>14572843</v>
       </c>
       <c r="AA47" s="1">
-        <f t="shared" ref="AA47" si="29">AVERAGE(W47:W51)</f>
+        <f t="shared" ref="AA47" si="30">AVERAGE(W47:W51)</f>
         <v>14572946</v>
       </c>
       <c r="AB47">
-        <f t="shared" ref="AB47" si="30">AA47-AA42</f>
+        <f t="shared" ref="AB47" si="31">AA47-AA42</f>
         <v>-335983.80000000075</v>
       </c>
     </row>

</xml_diff>